<commit_message>
Updated results and statistics
</commit_message>
<xml_diff>
--- a/data/new_posteriors/no_elementary_skills/complex_model/leak/constrained/results_model2a_leak_constrained.xlsx
+++ b/data/new_posteriors/no_elementary_skills/complex_model/leak/constrained/results_model2a_leak_constrained.xlsx
@@ -622,31 +622,31 @@
         <v>1.0</v>
       </c>
       <c r="E3" t="n" s="25">
-        <v>0.9989144119718087</v>
+        <v>0.9986191333468454</v>
       </c>
       <c r="F3" t="n" s="25">
-        <v>0.9999806645081193</v>
+        <v>0.9999210014873626</v>
       </c>
       <c r="G3" t="n" s="25">
-        <v>0.9999998624944785</v>
+        <v>0.9999926946991265</v>
       </c>
       <c r="H3" t="n" s="25">
-        <v>0.9989322938327848</v>
+        <v>0.9978836116696741</v>
       </c>
       <c r="I3" t="n" s="25">
-        <v>0.9999989848238333</v>
+        <v>0.9999655801119068</v>
       </c>
       <c r="J3" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999890136648715</v>
       </c>
       <c r="K3" t="n" s="25">
-        <v>0.9518491256237868</v>
+        <v>0.9044286429086849</v>
       </c>
       <c r="L3" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9143598979434332</v>
       </c>
       <c r="M3" t="n" s="25">
-        <v>1.0</v>
+        <v>0.12042941100991619</v>
       </c>
       <c r="N3" t="n" s="25">
         <v>0.5</v>
@@ -657,31 +657,31 @@
         <v>2.0</v>
       </c>
       <c r="E4" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F4" t="n" s="25">
-        <v>0.9999990823987623</v>
+        <v>0.9999955086148147</v>
       </c>
       <c r="G4" t="n" s="25">
-        <v>0.9999999999912884</v>
+        <v>0.9999999989250976</v>
       </c>
       <c r="H4" t="n" s="25">
-        <v>0.9998142743894936</v>
+        <v>0.999577198045728</v>
       </c>
       <c r="I4" t="n" s="25">
-        <v>0.9999999999961092</v>
+        <v>0.9999999996152397</v>
       </c>
       <c r="J4" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999908123</v>
       </c>
       <c r="K4" t="n" s="25">
-        <v>0.9996931334938806</v>
+        <v>0.9987903785670498</v>
       </c>
       <c r="L4" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999986530649053</v>
       </c>
       <c r="M4" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999942482729668</v>
       </c>
       <c r="N4" t="n" s="25">
         <v>0.5</v>
@@ -692,31 +692,31 @@
         <v>3.0</v>
       </c>
       <c r="E5" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F5" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G5" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H5" t="n" s="25">
-        <v>0.99998443095205</v>
+        <v>0.9999505548735174</v>
       </c>
       <c r="I5" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999657</v>
       </c>
       <c r="J5" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K5" t="n" s="25">
-        <v>0.9999945525612022</v>
+        <v>0.9999574938025837</v>
       </c>
       <c r="L5" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999942124</v>
       </c>
       <c r="M5" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999997791078</v>
       </c>
       <c r="N5" t="n" s="25">
         <v>0.5</v>
@@ -727,31 +727,31 @@
         <v>4.0</v>
       </c>
       <c r="E6" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F6" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G6" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H6" t="n" s="25">
-        <v>0.9999895610288345</v>
+        <v>0.9999648280181412</v>
       </c>
       <c r="I6" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999881</v>
       </c>
       <c r="J6" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K6" t="n" s="25">
-        <v>0.9999993488436147</v>
+        <v>0.9999926618203173</v>
       </c>
       <c r="L6" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999792</v>
       </c>
       <c r="M6" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999965665</v>
       </c>
       <c r="N6" t="n" s="25">
         <v>0.5</v>
@@ -762,31 +762,31 @@
         <v>5.0</v>
       </c>
       <c r="E7" t="n" s="25">
-        <v>0.9991868779273477</v>
+        <v>0.9989310716222465</v>
       </c>
       <c r="F7" t="n" s="25">
-        <v>0.9999993722586107</v>
+        <v>0.9999967835199167</v>
       </c>
       <c r="G7" t="n" s="25">
-        <v>0.9999999999927126</v>
+        <v>0.9999999990570784</v>
       </c>
       <c r="H7" t="n" s="25">
-        <v>0.9999701484324417</v>
+        <v>0.9999124083612652</v>
       </c>
       <c r="I7" t="n" s="25">
-        <v>0.9999999999999207</v>
+        <v>0.9999999999823012</v>
       </c>
       <c r="J7" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999747</v>
       </c>
       <c r="K7" t="n" s="25">
-        <v>0.9999803626688007</v>
+        <v>0.99985539587753</v>
       </c>
       <c r="L7" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999985300561</v>
       </c>
       <c r="M7" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999697090095</v>
       </c>
       <c r="N7" t="n" s="25">
         <v>0.5</v>
@@ -797,31 +797,31 @@
         <v>6.0</v>
       </c>
       <c r="E8" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F8" t="n" s="25">
-        <v>0.9999990823987623</v>
+        <v>0.9999955086148147</v>
       </c>
       <c r="G8" t="n" s="25">
-        <v>0.9999999999912884</v>
+        <v>0.9999999989250976</v>
       </c>
       <c r="H8" t="n" s="25">
-        <v>0.9995907801978414</v>
+        <v>0.9991825265854827</v>
       </c>
       <c r="I8" t="n" s="25">
-        <v>0.9999999999451366</v>
+        <v>0.9999999968081676</v>
       </c>
       <c r="J8" t="n" s="25">
-        <v>0.9999999999982191</v>
+        <v>0.9999999974064839</v>
       </c>
       <c r="K8" t="n" s="25">
-        <v>0.9751371412428526</v>
+        <v>0.9599597792651053</v>
       </c>
       <c r="L8" t="n" s="25">
-        <v>0.9974192073747251</v>
+        <v>0.983826055643527</v>
       </c>
       <c r="M8" t="n" s="25">
-        <v>0.9995761609582862</v>
+        <v>0.9846774843349747</v>
       </c>
       <c r="N8" t="n" s="25">
         <v>0.5</v>
@@ -832,31 +832,31 @@
         <v>7.0</v>
       </c>
       <c r="E9" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F9" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G9" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H9" t="n" s="25">
-        <v>0.9999935804766492</v>
+        <v>0.9999765240464018</v>
       </c>
       <c r="I9" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999961</v>
       </c>
       <c r="J9" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K9" t="n" s="25">
-        <v>0.9999999379889265</v>
+        <v>0.9999988572754733</v>
       </c>
       <c r="L9" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="M9" t="n" s="25">
-        <v>1.0</v>
+        <v>0.99999999999989</v>
       </c>
       <c r="N9" t="n" s="25">
         <v>0.5</v>
@@ -867,31 +867,31 @@
         <v>8.0</v>
       </c>
       <c r="E10" t="n" s="25">
-        <v>0.9990914510156967</v>
+        <v>0.9988209996328056</v>
       </c>
       <c r="F10" t="n" s="25">
-        <v>0.9999993618232316</v>
+        <v>0.9999967257208482</v>
       </c>
       <c r="G10" t="n" s="25">
-        <v>0.9999999999986967</v>
+        <v>0.999999999798686</v>
       </c>
       <c r="H10" t="n" s="25">
-        <v>0.9999371183044187</v>
+        <v>0.999833127704046</v>
       </c>
       <c r="I10" t="n" s="25">
-        <v>0.9999999999999517</v>
+        <v>0.9999999999908944</v>
       </c>
       <c r="J10" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999959</v>
       </c>
       <c r="K10" t="n" s="25">
-        <v>0.9999820816780681</v>
+        <v>0.9998826472857555</v>
       </c>
       <c r="L10" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999994704447</v>
       </c>
       <c r="M10" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999870140625</v>
       </c>
       <c r="N10" t="n" s="25">
         <v>0.5</v>
@@ -902,31 +902,31 @@
         <v>9.0</v>
       </c>
       <c r="E11" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F11" t="n" s="25">
-        <v>0.9999984521490705</v>
+        <v>0.9999931098114505</v>
       </c>
       <c r="G11" t="n" s="25">
-        <v>0.9999999947991584</v>
+        <v>0.9999997455340356</v>
       </c>
       <c r="H11" t="n" s="25">
-        <v>0.9999891264169046</v>
+        <v>0.9999637044948116</v>
       </c>
       <c r="I11" t="n" s="25">
-        <v>0.9999999999960442</v>
+        <v>0.9999999992456031</v>
       </c>
       <c r="J11" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999999999856057</v>
       </c>
       <c r="K11" t="n" s="25">
-        <v>0.9999855784331403</v>
+        <v>0.9998463155026578</v>
       </c>
       <c r="L11" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999419434114</v>
       </c>
       <c r="M11" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999982135839187</v>
       </c>
       <c r="N11" t="n" s="25">
         <v>0.5</v>
@@ -937,31 +937,31 @@
         <v>10.0</v>
       </c>
       <c r="E12" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F12" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G12" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H12" t="n" s="25">
-        <v>0.9999935804766492</v>
+        <v>0.9999765240464018</v>
       </c>
       <c r="I12" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999961</v>
       </c>
       <c r="J12" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K12" t="n" s="25">
-        <v>0.9999999379889265</v>
+        <v>0.9999988572754733</v>
       </c>
       <c r="L12" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="M12" t="n" s="25">
-        <v>1.0</v>
+        <v>0.99999999999989</v>
       </c>
       <c r="N12" t="n" s="25">
         <v>0.5</v>
@@ -972,31 +972,31 @@
         <v>11.0</v>
       </c>
       <c r="E13" t="n" s="25">
-        <v>0.9991855150308818</v>
+        <v>0.9989297175777208</v>
       </c>
       <c r="F13" t="n" s="25">
-        <v>0.9991587104338362</v>
+        <v>0.997910624876357</v>
       </c>
       <c r="G13" t="n" s="25">
-        <v>0.662132882802292</v>
+        <v>0.5715744219708038</v>
       </c>
       <c r="H13" t="n" s="25">
-        <v>0.999972604269044</v>
+        <v>0.9999004603275202</v>
       </c>
       <c r="I13" t="n" s="25">
-        <v>0.999999468785395</v>
+        <v>0.9999839773116124</v>
       </c>
       <c r="J13" t="n" s="25">
-        <v>1.0</v>
+        <v>0.2050477562724729</v>
       </c>
       <c r="K13" t="n" s="25">
-        <v>0.9999994566395787</v>
+        <v>0.9999835797376199</v>
       </c>
       <c r="L13" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999942604147299</v>
       </c>
       <c r="M13" t="n" s="25">
-        <v>1.0</v>
+        <v>0.0036726074710002428</v>
       </c>
       <c r="N13" t="n" s="25">
         <v>0.5</v>
@@ -1007,31 +1007,31 @@
         <v>12.0</v>
       </c>
       <c r="E14" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F14" t="n" s="25">
-        <v>0.9999861480188305</v>
+        <v>0.999956824851418</v>
       </c>
       <c r="G14" t="n" s="25">
-        <v>0.9701889156119111</v>
+        <v>0.9457320681121939</v>
       </c>
       <c r="H14" t="n" s="25">
-        <v>0.999984053391887</v>
+        <v>0.9999509197263996</v>
       </c>
       <c r="I14" t="n" s="25">
-        <v>0.9999781355902767</v>
+        <v>0.9998710605110718</v>
       </c>
       <c r="J14" t="n" s="25">
-        <v>0.9837825902400541</v>
+        <v>0.8698009573477861</v>
       </c>
       <c r="K14" t="n" s="25">
-        <v>0.9345280299237368</v>
+        <v>0.8974132993597048</v>
       </c>
       <c r="L14" t="n" s="25">
-        <v>0.920264453734804</v>
+        <v>0.6726143139198313</v>
       </c>
       <c r="M14" t="n" s="25">
-        <v>1.8544882892382612E-8</v>
+        <v>4.703036400116174E-10</v>
       </c>
       <c r="N14" t="n" s="25">
         <v>0.5</v>
@@ -1042,31 +1042,31 @@
         <v>13.0</v>
       </c>
       <c r="E15" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F15" t="n" s="25">
-        <v>0.9999960186635759</v>
+        <v>0.9999840408565418</v>
       </c>
       <c r="G15" t="n" s="25">
-        <v>0.9999911227536191</v>
+        <v>0.9998005026128187</v>
       </c>
       <c r="H15" t="n" s="25">
-        <v>0.9998142743894936</v>
+        <v>0.999577198045728</v>
       </c>
       <c r="I15" t="n" s="25">
-        <v>0.9999902587040193</v>
+        <v>0.9997727542362381</v>
       </c>
       <c r="J15" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9987658658401044</v>
       </c>
       <c r="K15" t="n" s="25">
-        <v>0.9831266592633527</v>
+        <v>0.9516437938118149</v>
       </c>
       <c r="L15" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9641375559413699</v>
       </c>
       <c r="M15" t="n" s="25">
-        <v>1.0</v>
+        <v>0.016413046639201186</v>
       </c>
       <c r="N15" t="n" s="25">
         <v>0.5</v>
@@ -1077,31 +1077,31 @@
         <v>14.0</v>
       </c>
       <c r="E16" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F16" t="n" s="25">
-        <v>0.9999967491131206</v>
+        <v>0.999987432274228</v>
       </c>
       <c r="G16" t="n" s="25">
-        <v>0.9999999949239186</v>
+        <v>0.9999998867852191</v>
       </c>
       <c r="H16" t="n" s="25">
-        <v>0.9999972740434746</v>
+        <v>0.9999888171869721</v>
       </c>
       <c r="I16" t="n" s="25">
-        <v>0.9999999999999977</v>
+        <v>0.9999999999994588</v>
       </c>
       <c r="J16" t="n" s="25">
-        <v>0.9999999999998826</v>
+        <v>0.9999999997357227</v>
       </c>
       <c r="K16" t="n" s="25">
-        <v>0.9999999445660884</v>
+        <v>0.9999988927029109</v>
       </c>
       <c r="L16" t="n" s="25">
-        <v>0.9999999999952317</v>
+        <v>0.9999999929046264</v>
       </c>
       <c r="M16" t="n" s="25">
-        <v>0.9999997982341461</v>
+        <v>0.9999764734461052</v>
       </c>
       <c r="N16" t="n" s="25">
         <v>0.5</v>
@@ -1112,31 +1112,31 @@
         <v>15.0</v>
       </c>
       <c r="E17" t="n" s="25">
-        <v>0.9991022957612626</v>
+        <v>0.9988334609079229</v>
       </c>
       <c r="F17" t="n" s="25">
-        <v>0.9999993911800813</v>
+        <v>0.99999685691061</v>
       </c>
       <c r="G17" t="n" s="25">
-        <v>0.9999999999990213</v>
+        <v>0.9999999998426593</v>
       </c>
       <c r="H17" t="n" s="25">
-        <v>0.9999379197837059</v>
+        <v>0.9998360248729632</v>
       </c>
       <c r="I17" t="n" s="25">
-        <v>0.9999999999999613</v>
+        <v>0.999999999992659</v>
       </c>
       <c r="J17" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999971</v>
       </c>
       <c r="K17" t="n" s="25">
-        <v>0.9999784053335432</v>
+        <v>0.9998683666212929</v>
       </c>
       <c r="L17" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999994817135</v>
       </c>
       <c r="M17" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999881428585</v>
       </c>
       <c r="N17" t="n" s="25">
         <v>0.5</v>
@@ -1147,31 +1147,31 @@
         <v>16.0</v>
       </c>
       <c r="E18" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F18" t="n" s="25">
-        <v>0.9999998196562523</v>
+        <v>0.9999989058735439</v>
       </c>
       <c r="G18" t="n" s="25">
-        <v>0.9999999999999974</v>
+        <v>0.9999999999990773</v>
       </c>
       <c r="H18" t="n" s="25">
-        <v>0.9999971598130695</v>
+        <v>0.9999884823730976</v>
       </c>
       <c r="I18" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="J18" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K18" t="n" s="25">
-        <v>0.9999999627394431</v>
+        <v>0.9999993006114953</v>
       </c>
       <c r="L18" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="M18" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999876</v>
       </c>
       <c r="N18" t="n" s="25">
         <v>0.5</v>
@@ -1182,31 +1182,31 @@
         <v>17.0</v>
       </c>
       <c r="E19" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F19" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G19" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H19" t="n" s="25">
-        <v>0.9999895610288345</v>
+        <v>0.9999648280181412</v>
       </c>
       <c r="I19" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999881</v>
       </c>
       <c r="J19" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K19" t="n" s="25">
-        <v>0.9999993488436147</v>
+        <v>0.9999926618203173</v>
       </c>
       <c r="L19" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999792</v>
       </c>
       <c r="M19" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999965665</v>
       </c>
       <c r="N19" t="n" s="25">
         <v>0.5</v>
@@ -1217,31 +1217,31 @@
         <v>18.0</v>
       </c>
       <c r="E20" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F20" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G20" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H20" t="n" s="25">
-        <v>0.99998443095205</v>
+        <v>0.9999505548735174</v>
       </c>
       <c r="I20" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999657</v>
       </c>
       <c r="J20" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K20" t="n" s="25">
-        <v>0.9999945525612022</v>
+        <v>0.9999574938025837</v>
       </c>
       <c r="L20" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999942124</v>
       </c>
       <c r="M20" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999997791078</v>
       </c>
       <c r="N20" t="n" s="25">
         <v>0.5</v>
@@ -1252,31 +1252,31 @@
         <v>19.0</v>
       </c>
       <c r="E21" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F21" t="n" s="25">
-        <v>0.9999998196562523</v>
+        <v>0.9999989058735439</v>
       </c>
       <c r="G21" t="n" s="25">
-        <v>0.9999999999999974</v>
+        <v>0.9999999999990773</v>
       </c>
       <c r="H21" t="n" s="25">
-        <v>0.9999981882542569</v>
+        <v>0.999992121572693</v>
       </c>
       <c r="I21" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="J21" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K21" t="n" s="25">
-        <v>0.999999996025087</v>
+        <v>0.9999998853821509</v>
       </c>
       <c r="L21" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="M21" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="N21" t="n" s="25">
         <v>0.5</v>
@@ -1287,31 +1287,31 @@
         <v>20.0</v>
       </c>
       <c r="E22" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F22" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G22" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H22" t="n" s="25">
-        <v>0.999989976051864</v>
+        <v>0.9999658351119862</v>
       </c>
       <c r="I22" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999885</v>
       </c>
       <c r="J22" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K22" t="n" s="25">
-        <v>0.9999994187414833</v>
+        <v>0.9999930286298917</v>
       </c>
       <c r="L22" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999706</v>
       </c>
       <c r="M22" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999950778</v>
       </c>
       <c r="N22" t="n" s="25">
         <v>0.5</v>
@@ -1322,31 +1322,31 @@
         <v>21.0</v>
       </c>
       <c r="E23" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F23" t="n" s="25">
-        <v>0.9999998196562523</v>
+        <v>0.9999989058735439</v>
       </c>
       <c r="G23" t="n" s="25">
-        <v>0.9999999999999974</v>
+        <v>0.9999999999990773</v>
       </c>
       <c r="H23" t="n" s="25">
-        <v>0.99999556166843</v>
+        <v>0.9999832222566263</v>
       </c>
       <c r="I23" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999993</v>
       </c>
       <c r="J23" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K23" t="n" s="25">
-        <v>0.9999996507333352</v>
+        <v>0.9999957329476131</v>
       </c>
       <c r="L23" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999973</v>
       </c>
       <c r="M23" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999994413</v>
       </c>
       <c r="N23" t="n" s="25">
         <v>0.5</v>
@@ -1357,31 +1357,31 @@
         <v>22.0</v>
       </c>
       <c r="E24" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F24" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G24" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H24" t="n" s="25">
-        <v>0.999989976051864</v>
+        <v>0.9999658351119862</v>
       </c>
       <c r="I24" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999885</v>
       </c>
       <c r="J24" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K24" t="n" s="25">
-        <v>0.9999994187414833</v>
+        <v>0.9999930286298917</v>
       </c>
       <c r="L24" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999706</v>
       </c>
       <c r="M24" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999950778</v>
       </c>
       <c r="N24" t="n" s="25">
         <v>0.5</v>
@@ -1392,31 +1392,31 @@
         <v>23.0</v>
       </c>
       <c r="E25" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F25" t="n" s="25">
-        <v>0.9999995692899719</v>
+        <v>0.9999976874904587</v>
       </c>
       <c r="G25" t="n" s="25">
-        <v>0.9999999999992263</v>
+        <v>0.999999999872747</v>
       </c>
       <c r="H25" t="n" s="25">
-        <v>0.99998443095205</v>
+        <v>0.9999505548735174</v>
       </c>
       <c r="I25" t="n" s="25">
-        <v>0.9999999999999972</v>
+        <v>0.9999999999990636</v>
       </c>
       <c r="J25" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="K25" t="n" s="25">
-        <v>0.9999878993211664</v>
+        <v>0.9999056839987414</v>
       </c>
       <c r="L25" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999999999843308</v>
       </c>
       <c r="M25" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999962454957</v>
       </c>
       <c r="N25" t="n" s="25">
         <v>0.5</v>
@@ -1427,31 +1427,31 @@
         <v>24.0</v>
       </c>
       <c r="E26" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F26" t="n" s="25">
-        <v>0.9882347584740286</v>
+        <v>0.974807694653337</v>
       </c>
       <c r="G26" t="n" s="25">
-        <v>0.8501996056959269</v>
+        <v>0.6803183272540965</v>
       </c>
       <c r="H26" t="n" s="25">
-        <v>0.9941323707917079</v>
+        <v>0.9888191705225906</v>
       </c>
       <c r="I26" t="n" s="25">
-        <v>0.9836940798670232</v>
+        <v>0.9514739183451673</v>
       </c>
       <c r="J26" t="n" s="25">
-        <v>1.0</v>
+        <v>0.34577378883102405</v>
       </c>
       <c r="K26" t="n" s="25">
-        <v>0.8458446683491476</v>
+        <v>0.8049266756262079</v>
       </c>
       <c r="L26" t="n" s="25">
-        <v>1.0</v>
+        <v>0.028475116943597084</v>
       </c>
       <c r="M26" t="n" s="25">
-        <v>1.0</v>
+        <v>1.2508725171551658E-10</v>
       </c>
       <c r="N26" t="n" s="25">
         <v>0.5</v>
@@ -1462,31 +1462,31 @@
         <v>25.0</v>
       </c>
       <c r="E27" t="n" s="25">
-        <v>0.9992837325783938</v>
+        <v>0.9990439143700659</v>
       </c>
       <c r="F27" t="n" s="25">
-        <v>0.999823830470837</v>
+        <v>0.9995162037817075</v>
       </c>
       <c r="G27" t="n" s="25">
-        <v>0.8018792065799122</v>
+        <v>0.7410146580729763</v>
       </c>
       <c r="H27" t="n" s="25">
-        <v>0.9999469055337381</v>
+        <v>0.9998403586359678</v>
       </c>
       <c r="I27" t="n" s="25">
-        <v>0.999837692933672</v>
+        <v>0.9992849151730738</v>
       </c>
       <c r="J27" t="n" s="25">
-        <v>0.12894987494326932</v>
+        <v>0.0273533578805018</v>
       </c>
       <c r="K27" t="n" s="25">
-        <v>0.9652099602691582</v>
+        <v>0.93683386905908</v>
       </c>
       <c r="L27" t="n" s="25">
-        <v>0.9494051967648652</v>
+        <v>0.6516442820129784</v>
       </c>
       <c r="M27" t="n" s="25">
-        <v>9.68771383930798E-12</v>
+        <v>2.307954116922455E-13</v>
       </c>
       <c r="N27" t="n" s="25">
         <v>0.5</v>
@@ -1497,31 +1497,31 @@
         <v>26.0</v>
       </c>
       <c r="E28" t="n" s="25">
-        <v>0.9991052860453463</v>
+        <v>0.9988363994420348</v>
       </c>
       <c r="F28" t="n" s="25">
-        <v>0.9999990856391697</v>
+        <v>0.9999955297369855</v>
       </c>
       <c r="G28" t="n" s="25">
-        <v>0.9999999999313559</v>
+        <v>0.999999993013435</v>
       </c>
       <c r="H28" t="n" s="25">
-        <v>0.9999428174729116</v>
+        <v>0.999845014259726</v>
       </c>
       <c r="I28" t="n" s="25">
-        <v>0.9999999999977818</v>
+        <v>0.9999999996651973</v>
       </c>
       <c r="J28" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999979097</v>
       </c>
       <c r="K28" t="n" s="25">
-        <v>0.9999680970923798</v>
+        <v>0.9997781381927695</v>
       </c>
       <c r="L28" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999861557681</v>
       </c>
       <c r="M28" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999997552305807</v>
       </c>
       <c r="N28" t="n" s="25">
         <v>0.5</v>
@@ -1532,31 +1532,31 @@
         <v>27.0</v>
       </c>
       <c r="E29" t="n" s="25">
-        <v>0.9987908017528341</v>
+        <v>0.9984807825459784</v>
       </c>
       <c r="F29" t="n" s="25">
-        <v>0.9999980651573475</v>
+        <v>0.9999913887212901</v>
       </c>
       <c r="G29" t="n" s="25">
-        <v>0.9999999992271364</v>
+        <v>0.9999999410373535</v>
       </c>
       <c r="H29" t="n" s="25">
-        <v>0.9989271966137127</v>
+        <v>0.9980883099357926</v>
       </c>
       <c r="I29" t="n" s="25">
-        <v>0.9999999864140503</v>
+        <v>0.9999995640332187</v>
       </c>
       <c r="J29" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999995633947013</v>
       </c>
       <c r="K29" t="n" s="25">
-        <v>0.9907598169824441</v>
+        <v>0.9815454524150033</v>
       </c>
       <c r="L29" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9944561065163015</v>
       </c>
       <c r="M29" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9905039380341577</v>
       </c>
       <c r="N29" t="n" s="25">
         <v>0.5</v>
@@ -1567,31 +1567,31 @@
         <v>28.0</v>
       </c>
       <c r="E30" t="n" s="25">
-        <v>0.9987908017528341</v>
+        <v>0.9984807825459784</v>
       </c>
       <c r="F30" t="n" s="25">
-        <v>0.9389583678874718</v>
+        <v>0.9094705019404349</v>
       </c>
       <c r="G30" t="n" s="25">
-        <v>0.3710355505442348</v>
+        <v>0.22498940905248738</v>
       </c>
       <c r="H30" t="n" s="25">
-        <v>0.9514495933189815</v>
+        <v>0.93618477487485</v>
       </c>
       <c r="I30" t="n" s="25">
-        <v>0.7413503745945411</v>
+        <v>0.5611103165591905</v>
       </c>
       <c r="J30" t="n" s="25">
-        <v>1.1196486324354682E-6</v>
+        <v>8.67603602493867E-8</v>
       </c>
       <c r="K30" t="n" s="25">
-        <v>0.6289790942122372</v>
+        <v>0.6066053151046354</v>
       </c>
       <c r="L30" t="n" s="25">
-        <v>1.1159050479343817E-5</v>
+        <v>4.702400104700051E-6</v>
       </c>
       <c r="M30" t="n" s="25">
-        <v>2.958357937121925E-24</v>
+        <v>2.8046291488412273E-25</v>
       </c>
       <c r="N30" t="n" s="25">
         <v>0.5</v>
@@ -1602,31 +1602,31 @@
         <v>29.0</v>
       </c>
       <c r="E31" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F31" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G31" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H31" t="n" s="25">
-        <v>0.9999933120295676</v>
+        <v>0.9999758232052484</v>
       </c>
       <c r="I31" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999999999999996</v>
       </c>
       <c r="J31" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K31" t="n" s="25">
-        <v>0.999999930531562</v>
+        <v>0.999998797134705</v>
       </c>
       <c r="L31" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="M31" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999233</v>
       </c>
       <c r="N31" t="n" s="25">
         <v>0.5</v>
@@ -1637,31 +1637,31 @@
         <v>30.0</v>
       </c>
       <c r="E32" t="n" s="25">
-        <v>0.9987908017528341</v>
+        <v>0.9984807825459784</v>
       </c>
       <c r="F32" t="n" s="25">
-        <v>0.9166419531470323</v>
+        <v>0.8868281515313045</v>
       </c>
       <c r="G32" t="n" s="25">
-        <v>0.08935153912123808</v>
+        <v>0.05709493719522227</v>
       </c>
       <c r="H32" t="n" s="25">
-        <v>0.9420076549231827</v>
+        <v>0.9271382119617537</v>
       </c>
       <c r="I32" t="n" s="25">
-        <v>0.5890004362739563</v>
+        <v>0.3899577918588311</v>
       </c>
       <c r="J32" t="n" s="25">
-        <v>1.5577002003059938E-8</v>
+        <v>1.6239671644213315E-9</v>
       </c>
       <c r="K32" t="n" s="25">
-        <v>0.6289755151517269</v>
+        <v>0.6066026348312759</v>
       </c>
       <c r="L32" t="n" s="25">
-        <v>2.511901554749694E-6</v>
+        <v>1.040656999909114E-6</v>
       </c>
       <c r="M32" t="n" s="25">
-        <v>3.11938804825768E-26</v>
+        <v>3.6740983992711495E-27</v>
       </c>
       <c r="N32" t="n" s="25">
         <v>0.5</v>
@@ -1672,31 +1672,31 @@
         <v>31.0</v>
       </c>
       <c r="E33" t="n" s="25">
-        <v>0.02591560888984709</v>
+        <v>0.02543368028981312</v>
       </c>
       <c r="F33" t="n" s="25">
-        <v>9.786150394826508E-5</v>
+        <v>8.33994093177786E-5</v>
       </c>
       <c r="G33" t="n" s="25">
-        <v>2.6791661751008323E-8</v>
+        <v>1.9563724255671545E-8</v>
       </c>
       <c r="H33" t="n" s="25">
-        <v>6.090017373979438E-4</v>
+        <v>5.10006147185278E-4</v>
       </c>
       <c r="I33" t="n" s="25">
-        <v>6.298050185759009E-9</v>
+        <v>2.1409606118122494E-9</v>
       </c>
       <c r="J33" t="n" s="25">
-        <v>6.415358546800807E-19</v>
+        <v>1.1509948405232337E-19</v>
       </c>
       <c r="K33" t="n" s="25">
-        <v>1.3707762280393096E-6</v>
+        <v>9.531490672167894E-7</v>
       </c>
       <c r="L33" t="n" s="25">
-        <v>9.776321363047916E-18</v>
+        <v>1.6546118928528543E-18</v>
       </c>
       <c r="M33" t="n" s="25">
-        <v>1.433915625866551E-38</v>
+        <v>1.3286214966730653E-39</v>
       </c>
       <c r="N33" t="n" s="25">
         <v>0.5</v>
@@ -1707,31 +1707,31 @@
         <v>32.0</v>
       </c>
       <c r="E34" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F34" t="n" s="25">
-        <v>0.9819609413641635</v>
+        <v>0.9660997502721836</v>
       </c>
       <c r="G34" t="n" s="25">
-        <v>0.18178003084876074</v>
+        <v>0.1360134941674401</v>
       </c>
       <c r="H34" t="n" s="25">
-        <v>0.9943397705692603</v>
+        <v>0.9891000947219253</v>
       </c>
       <c r="I34" t="n" s="25">
-        <v>0.981514963075046</v>
+        <v>0.9499946226636489</v>
       </c>
       <c r="J34" t="n" s="25">
-        <v>6.253540296617607E-6</v>
+        <v>1.175351809800874E-6</v>
       </c>
       <c r="K34" t="n" s="25">
-        <v>0.848204179536779</v>
+        <v>0.8051306034699912</v>
       </c>
       <c r="L34" t="n" s="25">
-        <v>0.004365498820730051</v>
+        <v>8.915846250541394E-4</v>
       </c>
       <c r="M34" t="n" s="25">
-        <v>2.12604849363419E-21</v>
+        <v>1.6784511216995148E-22</v>
       </c>
       <c r="N34" t="n" s="25">
         <v>0.5</v>
@@ -1742,31 +1742,31 @@
         <v>33.0</v>
       </c>
       <c r="E35" t="n" s="25">
-        <v>0.0030008732512320667</v>
+        <v>0.002965864031834444</v>
       </c>
       <c r="F35" t="n" s="25">
-        <v>6.933203655322773E-7</v>
+        <v>6.052606136728868E-7</v>
       </c>
       <c r="G35" t="n" s="25">
-        <v>1.103787617221983E-10</v>
+        <v>7.231366576956212E-11</v>
       </c>
       <c r="H35" t="n" s="25">
-        <v>1.0159851604464222E-6</v>
+        <v>8.747802828896881E-7</v>
       </c>
       <c r="I35" t="n" s="25">
-        <v>3.6368439604658647E-16</v>
+        <v>1.560741117898589E-16</v>
       </c>
       <c r="J35" t="n" s="25">
-        <v>1.1272544526930307E-28</v>
+        <v>2.208603632996956E-29</v>
       </c>
       <c r="K35" t="n" s="25">
-        <v>1.995571345401733E-11</v>
+        <v>1.7046037233668285E-11</v>
       </c>
       <c r="L35" t="n" s="25">
-        <v>9.343371020942581E-30</v>
+        <v>4.0953401154537584E-30</v>
       </c>
       <c r="M35" t="n" s="25">
-        <v>3.6631916508904305E-53</v>
+        <v>7.525524365023485E-54</v>
       </c>
       <c r="N35" t="n" s="25">
         <v>0.5</v>
@@ -1777,31 +1777,31 @@
         <v>34.0</v>
       </c>
       <c r="E36" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F36" t="n" s="25">
-        <v>0.9819609413641635</v>
+        <v>0.9660997502721836</v>
       </c>
       <c r="G36" t="n" s="25">
-        <v>0.18177945350846686</v>
+        <v>0.1360132560042527</v>
       </c>
       <c r="H36" t="n" s="25">
-        <v>0.9917169487612278</v>
+        <v>0.9850445633666501</v>
       </c>
       <c r="I36" t="n" s="25">
-        <v>0.9815082250157697</v>
+        <v>0.9499857398595162</v>
       </c>
       <c r="J36" t="n" s="25">
-        <v>2.501425504305147E-6</v>
+        <v>4.701410554689514E-7</v>
       </c>
       <c r="K36" t="n" s="25">
-        <v>0.6971051531045412</v>
+        <v>0.6696803375782686</v>
       </c>
       <c r="L36" t="n" s="25">
-        <v>1.5185665951317057E-4</v>
+        <v>5.997543858621399E-5</v>
       </c>
       <c r="M36" t="n" s="25">
-        <v>3.297816175103146E-24</v>
+        <v>5.0252523865497E-25</v>
       </c>
       <c r="N36" t="n" s="25">
         <v>0.5</v>
@@ -1812,31 +1812,31 @@
         <v>35.0</v>
       </c>
       <c r="E37" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F37" t="n" s="25">
-        <v>0.9819609413641635</v>
+        <v>0.9660997502721836</v>
       </c>
       <c r="G37" t="n" s="25">
-        <v>0.18178003084876074</v>
+        <v>0.1360134941674401</v>
       </c>
       <c r="H37" t="n" s="25">
-        <v>0.9943397705692603</v>
+        <v>0.9891000947219253</v>
       </c>
       <c r="I37" t="n" s="25">
-        <v>0.981514963075046</v>
+        <v>0.9499946226636489</v>
       </c>
       <c r="J37" t="n" s="25">
-        <v>6.253540296617607E-6</v>
+        <v>1.175351809800874E-6</v>
       </c>
       <c r="K37" t="n" s="25">
-        <v>0.848204179536779</v>
+        <v>0.8051306034699912</v>
       </c>
       <c r="L37" t="n" s="25">
-        <v>0.004365498820730051</v>
+        <v>8.915846250541394E-4</v>
       </c>
       <c r="M37" t="n" s="25">
-        <v>2.12604849363419E-21</v>
+        <v>1.6784511216995148E-22</v>
       </c>
       <c r="N37" t="n" s="25">
         <v>0.5</v>
@@ -1847,31 +1847,31 @@
         <v>36.0</v>
       </c>
       <c r="E38" t="n" s="25">
-        <v>0.9991293780754704</v>
+        <v>0.9988636285584939</v>
       </c>
       <c r="F38" t="n" s="25">
-        <v>0.9966891208581652</v>
+        <v>0.9917420822874278</v>
       </c>
       <c r="G38" t="n" s="25">
-        <v>0.9304152325289426</v>
+        <v>0.7667702836719938</v>
       </c>
       <c r="H38" t="n" s="25">
-        <v>0.9993711315807773</v>
+        <v>0.9983623031712335</v>
       </c>
       <c r="I38" t="n" s="25">
-        <v>0.9994974084867698</v>
+        <v>0.9942775911283448</v>
       </c>
       <c r="J38" t="n" s="25">
-        <v>0.9975797536982997</v>
+        <v>0.913952451686745</v>
       </c>
       <c r="K38" t="n" s="25">
-        <v>0.9915247472852626</v>
+        <v>0.9704902739925261</v>
       </c>
       <c r="L38" t="n" s="25">
-        <v>0.9974414581080712</v>
+        <v>0.9594931771647617</v>
       </c>
       <c r="M38" t="n" s="25">
-        <v>4.343341801322696E-4</v>
+        <v>2.475412936136853E-6</v>
       </c>
       <c r="N38" t="n" s="25">
         <v>0.5</v>
@@ -1882,31 +1882,31 @@
         <v>37.0</v>
       </c>
       <c r="E39" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F39" t="n" s="25">
-        <v>0.9819609413641635</v>
+        <v>0.9660997502721836</v>
       </c>
       <c r="G39" t="n" s="25">
-        <v>0.18178003084876074</v>
+        <v>0.1360134941674401</v>
       </c>
       <c r="H39" t="n" s="25">
-        <v>0.9943397705692603</v>
+        <v>0.9891000947219253</v>
       </c>
       <c r="I39" t="n" s="25">
-        <v>0.981514963075046</v>
+        <v>0.9499946226636489</v>
       </c>
       <c r="J39" t="n" s="25">
-        <v>6.253540296617605E-6</v>
+        <v>1.1753518098008743E-6</v>
       </c>
       <c r="K39" t="n" s="25">
-        <v>0.848204179536779</v>
+        <v>0.8051306034699911</v>
       </c>
       <c r="L39" t="n" s="25">
-        <v>0.004365498820730053</v>
+        <v>8.915846250541398E-4</v>
       </c>
       <c r="M39" t="n" s="25">
-        <v>2.1260484936341924E-21</v>
+        <v>1.6784511216995143E-22</v>
       </c>
       <c r="N39" t="n" s="25">
         <v>0.5</v>
@@ -1917,31 +1917,31 @@
         <v>38.0</v>
       </c>
       <c r="E40" t="n" s="25">
-        <v>0.9989042766169554</v>
+        <v>0.9986078061912221</v>
       </c>
       <c r="F40" t="n" s="25">
-        <v>0.9403763422274848</v>
+        <v>0.9108847217394104</v>
       </c>
       <c r="G40" t="n" s="25">
-        <v>0.08161296292577559</v>
+        <v>0.05923966914128257</v>
       </c>
       <c r="H40" t="n" s="25">
-        <v>0.9778572181928092</v>
+        <v>0.9662298039142545</v>
       </c>
       <c r="I40" t="n" s="25">
-        <v>0.8605781694748724</v>
+        <v>0.7108115603429157</v>
       </c>
       <c r="J40" t="n" s="25">
-        <v>2.759597474617355E-8</v>
+        <v>4.960845025188856E-9</v>
       </c>
       <c r="K40" t="n" s="25">
-        <v>0.8324143879645487</v>
+        <v>0.7879733921978401</v>
       </c>
       <c r="L40" t="n" s="25">
-        <v>3.365974628216923E-4</v>
+        <v>6.471261788083177E-5</v>
       </c>
       <c r="M40" t="n" s="25">
-        <v>3.0158027657970884E-24</v>
+        <v>2.700575885360542E-25</v>
       </c>
       <c r="N40" t="n" s="25">
         <v>0.5</v>
@@ -1952,31 +1952,31 @@
         <v>39.0</v>
       </c>
       <c r="E41" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F41" t="n" s="25">
-        <v>0.9999949180621203</v>
+        <v>0.9999769159282433</v>
       </c>
       <c r="G41" t="n" s="25">
-        <v>0.9999999999202009</v>
+        <v>0.999999993689152</v>
       </c>
       <c r="H41" t="n" s="25">
-        <v>0.9999871974121638</v>
+        <v>0.9999532908281555</v>
       </c>
       <c r="I41" t="n" s="25">
-        <v>0.999999999999996</v>
+        <v>0.9999999999984804</v>
       </c>
       <c r="J41" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999979</v>
       </c>
       <c r="K41" t="n" s="25">
-        <v>0.9999998120957404</v>
+        <v>0.9999965381408976</v>
       </c>
       <c r="L41" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999963548</v>
       </c>
       <c r="M41" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999982597667</v>
       </c>
       <c r="N41" t="n" s="25">
         <v>0.5</v>
@@ -1987,31 +1987,31 @@
         <v>40.0</v>
       </c>
       <c r="E42" t="n" s="25">
-        <v>0.8008039454656973</v>
+        <v>0.7820418903230698</v>
       </c>
       <c r="F42" t="n" s="25">
-        <v>0.12998720068888842</v>
+        <v>0.10902563429833424</v>
       </c>
       <c r="G42" t="n" s="25">
-        <v>0.004992910385521377</v>
+        <v>0.002378127408455184</v>
       </c>
       <c r="H42" t="n" s="25">
-        <v>0.12440518432398799</v>
+        <v>0.10521889489726018</v>
       </c>
       <c r="I42" t="n" s="25">
-        <v>2.5109803780805036E-5</v>
+        <v>9.622699845725026E-6</v>
       </c>
       <c r="J42" t="n" s="25">
-        <v>6.277397890399693E-16</v>
+        <v>8.175475873390966E-17</v>
       </c>
       <c r="K42" t="n" s="25">
-        <v>2.6049465307576204E-4</v>
+        <v>2.1091482500122836E-4</v>
       </c>
       <c r="L42" t="n" s="25">
-        <v>7.746792471183714E-17</v>
+        <v>2.9200117342044226E-17</v>
       </c>
       <c r="M42" t="n" s="25">
-        <v>2.2598824048604298E-38</v>
+        <v>3.196173201848055E-39</v>
       </c>
       <c r="N42" t="n" s="25">
         <v>0.5</v>
@@ -2022,31 +2022,31 @@
         <v>41.0</v>
       </c>
       <c r="E43" t="n" s="25">
-        <v>0.9990507614475552</v>
+        <v>0.9987731216953856</v>
       </c>
       <c r="F43" t="n" s="25">
-        <v>0.9906897065595687</v>
+        <v>0.9812372456062255</v>
       </c>
       <c r="G43" t="n" s="25">
-        <v>0.2973393113168089</v>
+        <v>0.23361075981277132</v>
       </c>
       <c r="H43" t="n" s="25">
-        <v>0.9979961314854824</v>
+        <v>0.9956721097374371</v>
       </c>
       <c r="I43" t="n" s="25">
-        <v>0.9914998062122097</v>
+        <v>0.9758278163047206</v>
       </c>
       <c r="J43" t="n" s="25">
-        <v>7.136315122712216E-5</v>
+        <v>1.4370046111923615E-5</v>
       </c>
       <c r="K43" t="n" s="25">
-        <v>0.8724171372917806</v>
+        <v>0.8316887921553519</v>
       </c>
       <c r="L43" t="n" s="25">
-        <v>9.903311330508268E-4</v>
+        <v>3.617340844148538E-4</v>
       </c>
       <c r="M43" t="n" s="25">
-        <v>1.5670984608908203E-21</v>
+        <v>1.9264861835129398E-22</v>
       </c>
       <c r="N43" t="n" s="25">
         <v>0.5</v>
@@ -2057,31 +2057,31 @@
         <v>42.0</v>
       </c>
       <c r="E44" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F44" t="n" s="25">
-        <v>0.9831531230767567</v>
+        <v>0.9677247320202985</v>
       </c>
       <c r="G44" t="n" s="25">
-        <v>0.326407356928911</v>
+        <v>0.23019686569008233</v>
       </c>
       <c r="H44" t="n" s="25">
-        <v>0.9943397705692603</v>
+        <v>0.9891000947219253</v>
       </c>
       <c r="I44" t="n" s="25">
-        <v>0.9815303675147542</v>
+        <v>0.9500153138035281</v>
       </c>
       <c r="J44" t="n" s="25">
-        <v>3.4174538515359133E-4</v>
+        <v>3.4072147967449994E-5</v>
       </c>
       <c r="K44" t="n" s="25">
-        <v>0.848303540404921</v>
+        <v>0.8051939944398641</v>
       </c>
       <c r="L44" t="n" s="25">
-        <v>0.012372545158383538</v>
+        <v>0.002543173656036692</v>
       </c>
       <c r="M44" t="n" s="25">
-        <v>3.4648819768132463E-18</v>
+        <v>1.571090253911472E-19</v>
       </c>
       <c r="N44" t="n" s="25">
         <v>0.5</v>
@@ -2092,31 +2092,31 @@
         <v>43.0</v>
       </c>
       <c r="E45" t="n" s="25">
-        <v>0.9991022957612626</v>
+        <v>0.9988334609079229</v>
       </c>
       <c r="F45" t="n" s="25">
-        <v>0.9957081778617088</v>
+        <v>0.9905328465036265</v>
       </c>
       <c r="G45" t="n" s="25">
-        <v>0.3882999618621447</v>
+        <v>0.3102485912814747</v>
       </c>
       <c r="H45" t="n" s="25">
-        <v>0.9987312267716575</v>
+        <v>0.9971272146179644</v>
       </c>
       <c r="I45" t="n" s="25">
-        <v>0.9966027156923531</v>
+        <v>0.9893645074929908</v>
       </c>
       <c r="J45" t="n" s="25">
-        <v>2.605023940305579E-4</v>
+        <v>5.12470544758299E-5</v>
       </c>
       <c r="K45" t="n" s="25">
-        <v>0.8703047435135894</v>
+        <v>0.8277701066203408</v>
       </c>
       <c r="L45" t="n" s="25">
-        <v>0.024652020176219345</v>
+        <v>0.005083843902370538</v>
       </c>
       <c r="M45" t="n" s="25">
-        <v>3.6402210641366673E-19</v>
+        <v>2.298487946322416E-20</v>
       </c>
       <c r="N45" t="n" s="25">
         <v>0.5</v>
@@ -2127,31 +2127,31 @@
         <v>45.0</v>
       </c>
       <c r="E46" t="n" s="25">
-        <v>0.5744654985357933</v>
+        <v>0.5672243988443981</v>
       </c>
       <c r="F46" t="n" s="25">
-        <v>0.002258420352442836</v>
+        <v>0.001990167788586255</v>
       </c>
       <c r="G46" t="n" s="25">
-        <v>3.319968972113806E-10</v>
+        <v>2.4036918284242294E-10</v>
       </c>
       <c r="H46" t="n" s="25">
-        <v>0.0012067084543187006</v>
+        <v>0.00112439014397815</v>
       </c>
       <c r="I46" t="n" s="25">
-        <v>5.713148883879286E-17</v>
+        <v>3.993320570597527E-17</v>
       </c>
       <c r="J46" t="n" s="25">
-        <v>7.898706184925262E-42</v>
+        <v>4.393439248102189E-42</v>
       </c>
       <c r="K46" t="n" s="25">
-        <v>5.699576625404594E-9</v>
+        <v>5.215401406390229E-9</v>
       </c>
       <c r="L46" t="n" s="25">
-        <v>6.418772107621152E-36</v>
+        <v>4.606915151512079E-36</v>
       </c>
       <c r="M46" t="n" s="25">
-        <v>1.3425644521489974E-72</v>
+        <v>7.699374731557017E-73</v>
       </c>
       <c r="N46" t="n" s="25">
         <v>0.5</v>
@@ -2162,31 +2162,31 @@
         <v>46.0</v>
       </c>
       <c r="E47" t="n" s="25">
-        <v>0.8397380186856837</v>
+        <v>0.8217479978657533</v>
       </c>
       <c r="F47" t="n" s="25">
-        <v>0.17917132496787685</v>
+        <v>0.15136549715215417</v>
       </c>
       <c r="G47" t="n" s="25">
-        <v>0.0035167020843370365</v>
+        <v>0.0014293783008268034</v>
       </c>
       <c r="H47" t="n" s="25">
-        <v>0.1368743266460483</v>
+        <v>0.11715686137645144</v>
       </c>
       <c r="I47" t="n" s="25">
-        <v>3.967409038548407E-7</v>
+        <v>1.9614018695476569E-7</v>
       </c>
       <c r="J47" t="n" s="25">
-        <v>3.210254074810027E-20</v>
+        <v>4.467291989007104E-21</v>
       </c>
       <c r="K47" t="n" s="25">
-        <v>4.3951014723263857E-4</v>
+        <v>3.009797365276513E-4</v>
       </c>
       <c r="L47" t="n" s="25">
-        <v>1.284020960731065E-19</v>
+        <v>5.160406266484768E-20</v>
       </c>
       <c r="M47" t="n" s="25">
-        <v>1.6610973901266167E-42</v>
+        <v>2.2734573299323123E-43</v>
       </c>
       <c r="N47" t="n" s="25">
         <v>0.5</v>
@@ -2197,31 +2197,31 @@
         <v>47.0</v>
       </c>
       <c r="E48" t="n" s="25">
-        <v>0.7123877289715882</v>
+        <v>0.6969198995094696</v>
       </c>
       <c r="F48" t="n" s="25">
-        <v>0.03659298426612251</v>
+        <v>0.031333464643942294</v>
       </c>
       <c r="G48" t="n" s="25">
-        <v>3.100569714155724E-4</v>
+        <v>1.6347314780407326E-4</v>
       </c>
       <c r="H48" t="n" s="25">
-        <v>0.09386396964431457</v>
+        <v>0.07993556384647957</v>
       </c>
       <c r="I48" t="n" s="25">
-        <v>4.878099956186544E-6</v>
+        <v>1.9736745764611183E-6</v>
       </c>
       <c r="J48" t="n" s="25">
-        <v>2.1243814616707462E-16</v>
+        <v>3.107212079767951E-17</v>
       </c>
       <c r="K48" t="n" s="25">
-        <v>4.681157358465642E-5</v>
+        <v>3.8584542343708526E-5</v>
       </c>
       <c r="L48" t="n" s="25">
-        <v>2.443114485781658E-18</v>
+        <v>1.0003228457015875E-18</v>
       </c>
       <c r="M48" t="n" s="25">
-        <v>3.978218550848296E-39</v>
+        <v>6.254727853002377E-40</v>
       </c>
       <c r="N48" t="n" s="25">
         <v>0.5</v>
@@ -2232,31 +2232,31 @@
         <v>49.0</v>
       </c>
       <c r="E49" t="n" s="25">
-        <v>0.9987908017528341</v>
+        <v>0.9984807825459784</v>
       </c>
       <c r="F49" t="n" s="25">
-        <v>0.9153631892838021</v>
+        <v>0.8856384309288827</v>
       </c>
       <c r="G49" t="n" s="25">
-        <v>0.04305136742092847</v>
+        <v>0.030893706567753216</v>
       </c>
       <c r="H49" t="n" s="25">
-        <v>0.9420076549231827</v>
+        <v>0.9271382119617537</v>
       </c>
       <c r="I49" t="n" s="25">
-        <v>0.5889986048884246</v>
+        <v>0.3899564887186311</v>
       </c>
       <c r="J49" t="n" s="25">
-        <v>2.8042268195696514E-10</v>
+        <v>5.5383147747967103E-11</v>
       </c>
       <c r="K49" t="n" s="25">
-        <v>0.6289738006418275</v>
+        <v>0.606601350880938</v>
       </c>
       <c r="L49" t="n" s="25">
-        <v>8.791669796099726E-7</v>
+        <v>3.642301963433455E-7</v>
       </c>
       <c r="M49" t="n" s="25">
-        <v>1.913695489031191E-29</v>
+        <v>3.924793570503929E-30</v>
       </c>
       <c r="N49" t="n" s="25">
         <v>0.5</v>
@@ -2267,31 +2267,31 @@
         <v>50.0</v>
       </c>
       <c r="E50" t="n" s="25">
-        <v>0.8380853097229516</v>
+        <v>0.8230950839673713</v>
       </c>
       <c r="F50" t="n" s="25">
-        <v>0.1760350058450439</v>
+        <v>0.15042028274150648</v>
       </c>
       <c r="G50" t="n" s="25">
-        <v>1.1641081330387541E-4</v>
+        <v>8.221709563064639E-5</v>
       </c>
       <c r="H50" t="n" s="25">
-        <v>0.11393829103980715</v>
+        <v>0.10311251749902473</v>
       </c>
       <c r="I50" t="n" s="25">
-        <v>1.3857736440450305E-5</v>
+        <v>6.5895114272188075E-6</v>
       </c>
       <c r="J50" t="n" s="25">
-        <v>9.952088606768931E-20</v>
+        <v>2.4560157336651612E-20</v>
       </c>
       <c r="K50" t="n" s="25">
-        <v>0.0016827240318467362</v>
+        <v>0.0014922377628075942</v>
       </c>
       <c r="L50" t="n" s="25">
-        <v>1.8311904336860947E-16</v>
+        <v>8.770155402262554E-17</v>
       </c>
       <c r="M50" t="n" s="25">
-        <v>3.182511282446816E-42</v>
+        <v>8.278785765843811E-43</v>
       </c>
       <c r="N50" t="n" s="25">
         <v>0.5</v>
@@ -2302,31 +2302,31 @@
         <v>51.0</v>
       </c>
       <c r="E51" t="n" s="25">
-        <v>0.24333780637987096</v>
+        <v>0.2386717184271144</v>
       </c>
       <c r="F51" t="n" s="25">
-        <v>3.981027563220998E-4</v>
+        <v>3.487280934299658E-4</v>
       </c>
       <c r="G51" t="n" s="25">
-        <v>1.2150430238024933E-7</v>
+        <v>4.299397407777216E-8</v>
       </c>
       <c r="H51" t="n" s="25">
-        <v>4.7441917566603593E-4</v>
+        <v>4.100622872363407E-4</v>
       </c>
       <c r="I51" t="n" s="25">
-        <v>3.131821476306768E-19</v>
+        <v>2.2144350017671835E-19</v>
       </c>
       <c r="J51" t="n" s="25">
-        <v>6.96149223270923E-38</v>
+        <v>1.7479481385698686E-38</v>
       </c>
       <c r="K51" t="n" s="25">
-        <v>2.5668582402687254E-12</v>
+        <v>2.18109967163211E-12</v>
       </c>
       <c r="L51" t="n" s="25">
-        <v>1.45632508012006E-41</v>
+        <v>1.0393889378744969E-41</v>
       </c>
       <c r="M51" t="n" s="25">
-        <v>5.796071495307956E-68</v>
+        <v>1.686584220323611E-68</v>
       </c>
       <c r="N51" t="n" s="25">
         <v>0.5</v>
@@ -2337,31 +2337,31 @@
         <v>52.0</v>
       </c>
       <c r="E52" t="n" s="25">
-        <v>0.9990422737679753</v>
+        <v>0.9987632784005972</v>
       </c>
       <c r="F52" t="n" s="25">
-        <v>0.9781313745927115</v>
+        <v>0.9592714740627055</v>
       </c>
       <c r="G52" t="n" s="25">
-        <v>0.18177927936960941</v>
+        <v>0.13601318234576654</v>
       </c>
       <c r="H52" t="n" s="25">
-        <v>0.9907520775850214</v>
+        <v>0.9831793263953597</v>
       </c>
       <c r="I52" t="n" s="25">
-        <v>0.9766639606348924</v>
+        <v>0.9352215233515904</v>
       </c>
       <c r="J52" t="n" s="25">
-        <v>1.2136558128535984E-6</v>
+        <v>2.1246142306568578E-7</v>
       </c>
       <c r="K52" t="n" s="25">
-        <v>0.7079921250041061</v>
+        <v>0.6794655996676895</v>
       </c>
       <c r="L52" t="n" s="25">
-        <v>1.087671103017833E-4</v>
+        <v>4.013214078980563E-5</v>
       </c>
       <c r="M52" t="n" s="25">
-        <v>8.306337547665241E-25</v>
+        <v>1.1909236337549082E-25</v>
       </c>
       <c r="N52" t="n" s="25">
         <v>0.5</v>
@@ -2372,31 +2372,31 @@
         <v>53.0</v>
       </c>
       <c r="E53" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F53" t="n" s="25">
-        <v>0.9999904517203423</v>
+        <v>0.9999622905668358</v>
       </c>
       <c r="G53" t="n" s="25">
-        <v>0.999996284387409</v>
+        <v>0.9999157148445433</v>
       </c>
       <c r="H53" t="n" s="25">
-        <v>0.9999397701574421</v>
+        <v>0.9997990087396218</v>
       </c>
       <c r="I53" t="n" s="25">
-        <v>0.9999999719077352</v>
+        <v>0.9999972665244485</v>
       </c>
       <c r="J53" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999647086061151</v>
       </c>
       <c r="K53" t="n" s="25">
-        <v>0.9978918435171488</v>
+        <v>0.9858609682079931</v>
       </c>
       <c r="L53" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9963610250955138</v>
       </c>
       <c r="M53" t="n" s="25">
-        <v>1.0</v>
+        <v>0.5506697948811609</v>
       </c>
       <c r="N53" t="n" s="25">
         <v>0.5</v>
@@ -2407,31 +2407,31 @@
         <v>54.0</v>
       </c>
       <c r="E54" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F54" t="n" s="25">
-        <v>0.9999971392243888</v>
+        <v>0.999988679637035</v>
       </c>
       <c r="G54" t="n" s="25">
-        <v>0.9999999176023243</v>
+        <v>0.9999980845088224</v>
       </c>
       <c r="H54" t="n" s="25">
-        <v>0.99999556166843</v>
+        <v>0.9999832222566263</v>
       </c>
       <c r="I54" t="n" s="25">
-        <v>0.9999999999979815</v>
+        <v>0.999999999640403</v>
       </c>
       <c r="J54" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999999987192208</v>
       </c>
       <c r="K54" t="n" s="25">
-        <v>0.9999936183774181</v>
+        <v>0.9999223481639812</v>
       </c>
       <c r="L54" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999989821467534</v>
       </c>
       <c r="M54" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999231654438954</v>
       </c>
       <c r="N54" t="n" s="25">
         <v>0.5</v>
@@ -2442,31 +2442,31 @@
         <v>55.0</v>
       </c>
       <c r="E55" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F55" t="n" s="25">
-        <v>0.9999074241126653</v>
+        <v>0.9997355716532327</v>
       </c>
       <c r="G55" t="n" s="25">
-        <v>0.9316352658369755</v>
+        <v>0.8844336591301855</v>
       </c>
       <c r="H55" t="n" s="25">
-        <v>0.9999689506090006</v>
+        <v>0.9999016235253874</v>
       </c>
       <c r="I55" t="n" s="25">
-        <v>0.999978347588182</v>
+        <v>0.9997520960124688</v>
       </c>
       <c r="J55" t="n" s="25">
-        <v>0.9629332341216026</v>
+        <v>0.752429287167356</v>
       </c>
       <c r="K55" t="n" s="25">
-        <v>0.9972455515662343</v>
+        <v>0.9852885896413601</v>
       </c>
       <c r="L55" t="n" s="25">
-        <v>0.9995160872439349</v>
+        <v>0.9906518562593147</v>
       </c>
       <c r="M55" t="n" s="25">
-        <v>2.0262555536500452E-5</v>
+        <v>2.5583625344278786E-7</v>
       </c>
       <c r="N55" t="n" s="25">
         <v>0.5</v>
@@ -2477,31 +2477,31 @@
         <v>56.0</v>
       </c>
       <c r="E56" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F56" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G56" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H56" t="n" s="25">
-        <v>0.9999895610288345</v>
+        <v>0.9999648280181412</v>
       </c>
       <c r="I56" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999881</v>
       </c>
       <c r="J56" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K56" t="n" s="25">
-        <v>0.9999993488436147</v>
+        <v>0.9999926618203173</v>
       </c>
       <c r="L56" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999999792</v>
       </c>
       <c r="M56" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999965665</v>
       </c>
       <c r="N56" t="n" s="25">
         <v>0.5</v>
@@ -2512,31 +2512,31 @@
         <v>57.0</v>
       </c>
       <c r="E57" t="n" s="25">
-        <v>0.9992923581596833</v>
+        <v>0.9990541090525831</v>
       </c>
       <c r="F57" t="n" s="25">
-        <v>0.9999417213925367</v>
+        <v>0.9998113523691222</v>
       </c>
       <c r="G57" t="n" s="25">
-        <v>0.9974476043290684</v>
+        <v>0.9824401557127136</v>
       </c>
       <c r="H57" t="n" s="25">
-        <v>0.9999318124283988</v>
+        <v>0.9998072493421575</v>
       </c>
       <c r="I57" t="n" s="25">
-        <v>0.9999876578494407</v>
+        <v>0.9998063324225566</v>
       </c>
       <c r="J57" t="n" s="25">
-        <v>0.9999152906764968</v>
+        <v>0.9973146364222572</v>
       </c>
       <c r="K57" t="n" s="25">
-        <v>0.9297013322578881</v>
+        <v>0.8871853373127415</v>
       </c>
       <c r="L57" t="n" s="25">
-        <v>0.935824700262438</v>
+        <v>0.7379541339831257</v>
       </c>
       <c r="M57" t="n" s="25">
-        <v>3.101634079000873E-5</v>
+        <v>5.866514731463383E-7</v>
       </c>
       <c r="N57" t="n" s="25">
         <v>0.5</v>
@@ -2547,31 +2547,31 @@
         <v>58.0</v>
       </c>
       <c r="E58" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F58" t="n" s="25">
-        <v>0.9999990823987623</v>
+        <v>0.9999955086148147</v>
       </c>
       <c r="G58" t="n" s="25">
-        <v>0.9999999999912884</v>
+        <v>0.9999999989250976</v>
       </c>
       <c r="H58" t="n" s="25">
-        <v>0.9995907801978414</v>
+        <v>0.9991825265854827</v>
       </c>
       <c r="I58" t="n" s="25">
-        <v>0.9999999999451366</v>
+        <v>0.9999999968081676</v>
       </c>
       <c r="J58" t="n" s="25">
-        <v>0.9999999999982191</v>
+        <v>0.9999999974064839</v>
       </c>
       <c r="K58" t="n" s="25">
-        <v>0.9751371412428526</v>
+        <v>0.9599597792651053</v>
       </c>
       <c r="L58" t="n" s="25">
-        <v>0.9974192073747251</v>
+        <v>0.983826055643527</v>
       </c>
       <c r="M58" t="n" s="25">
-        <v>0.9995761609582862</v>
+        <v>0.9846774843349747</v>
       </c>
       <c r="N58" t="n" s="25">
         <v>0.5</v>
@@ -2582,31 +2582,31 @@
         <v>59.0</v>
       </c>
       <c r="E59" t="n" s="25">
-        <v>0.9990914510156967</v>
+        <v>0.9988209996328056</v>
       </c>
       <c r="F59" t="n" s="25">
-        <v>0.9998132900645293</v>
+        <v>0.9993196851353778</v>
       </c>
       <c r="G59" t="n" s="25">
-        <v>0.999998821116695</v>
+        <v>0.9999538620421178</v>
       </c>
       <c r="H59" t="n" s="25">
-        <v>0.999215089347457</v>
+        <v>0.9982190129948602</v>
       </c>
       <c r="I59" t="n" s="25">
-        <v>0.9999996257663858</v>
+        <v>0.9999836575354792</v>
       </c>
       <c r="J59" t="n" s="25">
-        <v>0.9999999836553958</v>
+        <v>0.9999963017407149</v>
       </c>
       <c r="K59" t="n" s="25">
-        <v>0.9482987172833985</v>
+        <v>0.900653928478895</v>
       </c>
       <c r="L59" t="n" s="25">
-        <v>0.9753296974278768</v>
+        <v>0.8957198218271953</v>
       </c>
       <c r="M59" t="n" s="25">
-        <v>0.5054785886363874</v>
+        <v>0.019848347674414298</v>
       </c>
       <c r="N59" t="n" s="25">
         <v>0.5</v>
@@ -2617,31 +2617,31 @@
         <v>60.0</v>
       </c>
       <c r="E60" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F60" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G60" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H60" t="n" s="25">
-        <v>0.9999628075193137</v>
+        <v>0.9998979362688206</v>
       </c>
       <c r="I60" t="n" s="25">
-        <v>0.9999999999999988</v>
+        <v>0.9999999999996896</v>
       </c>
       <c r="J60" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999999999999999</v>
       </c>
       <c r="K60" t="n" s="25">
-        <v>0.9994964231498145</v>
+        <v>0.9984064410760951</v>
       </c>
       <c r="L60" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999997975070206</v>
       </c>
       <c r="M60" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999996150104454</v>
       </c>
       <c r="N60" t="n" s="25">
         <v>0.5</v>
@@ -2652,31 +2652,31 @@
         <v>61.0</v>
       </c>
       <c r="E61" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F61" t="n" s="25">
-        <v>0.9999769638830568</v>
+        <v>0.9999177842550951</v>
       </c>
       <c r="G61" t="n" s="25">
-        <v>0.999999540157244</v>
+        <v>0.9999904175560466</v>
       </c>
       <c r="H61" t="n" s="25">
-        <v>0.9999689506090006</v>
+        <v>0.9999016235253874</v>
       </c>
       <c r="I61" t="n" s="25">
-        <v>0.9999999999111292</v>
+        <v>0.9999999903047949</v>
       </c>
       <c r="J61" t="n" s="25">
-        <v>0.9999999953823512</v>
+        <v>0.9999992332831183</v>
       </c>
       <c r="K61" t="n" s="25">
-        <v>0.999918845286931</v>
+        <v>0.9993746905600268</v>
       </c>
       <c r="L61" t="n" s="25">
-        <v>0.9999926651801796</v>
+        <v>0.9997784248841499</v>
       </c>
       <c r="M61" t="n" s="25">
-        <v>0.9989299833739479</v>
+        <v>0.9484219585825963</v>
       </c>
       <c r="N61" t="n" s="25">
         <v>0.5</v>
@@ -2687,31 +2687,31 @@
         <v>62.0</v>
       </c>
       <c r="E62" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F62" t="n" s="25">
-        <v>0.9999975114725684</v>
+        <v>0.9999896485488656</v>
       </c>
       <c r="G62" t="n" s="25">
-        <v>0.9999998956840445</v>
+        <v>0.9999966883966117</v>
       </c>
       <c r="H62" t="n" s="25">
-        <v>0.99998443095205</v>
+        <v>0.9999505548735174</v>
       </c>
       <c r="I62" t="n" s="25">
-        <v>0.9999999998980724</v>
+        <v>0.9999999877259214</v>
       </c>
       <c r="J62" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999999025255536</v>
       </c>
       <c r="K62" t="n" s="25">
-        <v>0.9998930392269068</v>
+        <v>0.9991793575739556</v>
       </c>
       <c r="L62" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9997984018009753</v>
       </c>
       <c r="M62" t="n" s="25">
-        <v>1.0</v>
+        <v>0.993662049410392</v>
       </c>
       <c r="N62" t="n" s="25">
         <v>0.5</v>
@@ -2722,31 +2722,31 @@
         <v>63.0</v>
       </c>
       <c r="E63" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F63" t="n" s="25">
-        <v>0.9999908665684427</v>
+        <v>0.9999620183533</v>
       </c>
       <c r="G63" t="n" s="25">
-        <v>0.999999994514253</v>
+        <v>0.9999997125136051</v>
       </c>
       <c r="H63" t="n" s="25">
-        <v>0.9999512294725693</v>
+        <v>0.9998569458546089</v>
       </c>
       <c r="I63" t="n" s="25">
-        <v>0.9999999999708159</v>
+        <v>0.9999999959192523</v>
       </c>
       <c r="J63" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999886154324</v>
       </c>
       <c r="K63" t="n" s="25">
-        <v>0.9990856830196468</v>
+        <v>0.9957109684135897</v>
       </c>
       <c r="L63" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9993253406230515</v>
       </c>
       <c r="M63" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9981027034867918</v>
       </c>
       <c r="N63" t="n" s="25">
         <v>0.5</v>
@@ -2757,31 +2757,31 @@
         <v>64.0</v>
       </c>
       <c r="E64" t="n" s="25">
-        <v>0.9990914510156967</v>
+        <v>0.9988209996328056</v>
       </c>
       <c r="F64" t="n" s="25">
-        <v>0.9999993618232316</v>
+        <v>0.9999967257208482</v>
       </c>
       <c r="G64" t="n" s="25">
-        <v>0.9999999999986967</v>
+        <v>0.999999999798686</v>
       </c>
       <c r="H64" t="n" s="25">
-        <v>0.9999036795498427</v>
+        <v>0.9997616888408106</v>
       </c>
       <c r="I64" t="n" s="25">
-        <v>0.9999999999998141</v>
+        <v>0.9999999999728588</v>
       </c>
       <c r="J64" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999998667</v>
       </c>
       <c r="K64" t="n" s="25">
-        <v>0.9998324012392663</v>
+        <v>0.999287700146401</v>
       </c>
       <c r="L64" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999998918053807</v>
       </c>
       <c r="M64" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999994069485726</v>
       </c>
       <c r="N64" t="n" s="25">
         <v>0.5</v>
@@ -2792,31 +2792,31 @@
         <v>65.0</v>
       </c>
       <c r="E65" t="n" s="25">
-        <v>0.9991945711121792</v>
+        <v>0.9989401470167044</v>
       </c>
       <c r="F65" t="n" s="25">
-        <v>0.9999779074381105</v>
+        <v>0.9999175520510926</v>
       </c>
       <c r="G65" t="n" s="25">
-        <v>0.9999998312946454</v>
+        <v>0.9999939296527675</v>
       </c>
       <c r="H65" t="n" s="25">
-        <v>0.999970528955589</v>
+        <v>0.9999045845182468</v>
       </c>
       <c r="I65" t="n" s="25">
-        <v>0.9999999990985458</v>
+        <v>0.9999998859063091</v>
       </c>
       <c r="J65" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999997490298316</v>
       </c>
       <c r="K65" t="n" s="25">
-        <v>0.9998481053986551</v>
+        <v>0.9986361147429343</v>
       </c>
       <c r="L65" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9996975325507751</v>
       </c>
       <c r="M65" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9986712823985984</v>
       </c>
       <c r="N65" t="n" s="25">
         <v>0.5</v>
@@ -2827,31 +2827,31 @@
         <v>66.0</v>
       </c>
       <c r="E66" t="n" s="25">
-        <v>0.9904290733712912</v>
+        <v>0.988313524527594</v>
       </c>
       <c r="F66" t="n" s="25">
-        <v>0.6795561316188591</v>
+        <v>0.6224225542133676</v>
       </c>
       <c r="G66" t="n" s="25">
-        <v>0.01862076275982707</v>
+        <v>0.011607680502976517</v>
       </c>
       <c r="H66" t="n" s="25">
-        <v>0.6369056464396134</v>
+        <v>0.5985030454861379</v>
       </c>
       <c r="I66" t="n" s="25">
-        <v>0.10381173511266484</v>
+        <v>0.047965118491234776</v>
       </c>
       <c r="J66" t="n" s="25">
-        <v>1.2238806570723983E-10</v>
+        <v>1.403580241237713E-11</v>
       </c>
       <c r="K66" t="n" s="25">
-        <v>0.1541469166029742</v>
+        <v>0.14056857485537422</v>
       </c>
       <c r="L66" t="n" s="25">
-        <v>5.540399224778618E-9</v>
+        <v>2.2634585556271504E-9</v>
       </c>
       <c r="M66" t="n" s="25">
-        <v>2.9518513140989205E-29</v>
+        <v>3.898253874219752E-30</v>
       </c>
       <c r="N66" t="n" s="25">
         <v>0.5</v>
@@ -2862,31 +2862,31 @@
         <v>67.0</v>
       </c>
       <c r="E67" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F67" t="n" s="25">
-        <v>0.999837940374962</v>
+        <v>0.9995756731114127</v>
       </c>
       <c r="G67" t="n" s="25">
-        <v>0.7098626240287235</v>
+        <v>0.6615100663730558</v>
       </c>
       <c r="H67" t="n" s="25">
-        <v>0.9999861009548352</v>
+        <v>0.9999503396167166</v>
       </c>
       <c r="I67" t="n" s="25">
-        <v>0.9999957683968997</v>
+        <v>0.9999132401972662</v>
       </c>
       <c r="J67" t="n" s="25">
-        <v>0.0785058791607004</v>
+        <v>0.027848427032300255</v>
       </c>
       <c r="K67" t="n" s="25">
-        <v>0.9999175134447953</v>
+        <v>0.9987965313852237</v>
       </c>
       <c r="L67" t="n" s="25">
-        <v>0.9999921330885142</v>
+        <v>0.9995227323840998</v>
       </c>
       <c r="M67" t="n" s="25">
-        <v>5.74863332103366E-7</v>
+        <v>1.351465319432256E-8</v>
       </c>
       <c r="N67" t="n" s="25">
         <v>0.5</v>
@@ -2897,31 +2897,31 @@
         <v>68.0</v>
       </c>
       <c r="E68" t="n" s="25">
-        <v>0.999081045291687</v>
+        <v>0.9988089090238188</v>
       </c>
       <c r="F68" t="n" s="25">
-        <v>0.9995566379641986</v>
+        <v>0.9986804262058971</v>
       </c>
       <c r="G68" t="n" s="25">
-        <v>0.9999531534946061</v>
+        <v>0.9991473578609247</v>
       </c>
       <c r="H68" t="n" s="25">
-        <v>0.9997560531114325</v>
+        <v>0.9993517185998465</v>
       </c>
       <c r="I68" t="n" s="25">
-        <v>0.9999985443098466</v>
+        <v>0.9999429408690133</v>
       </c>
       <c r="J68" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999950720510542</v>
       </c>
       <c r="K68" t="n" s="25">
-        <v>0.994917026789872</v>
+        <v>0.9817628554630099</v>
       </c>
       <c r="L68" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9770321724061943</v>
       </c>
       <c r="M68" t="n" s="25">
-        <v>1.0</v>
+        <v>0.2551334629199231</v>
       </c>
       <c r="N68" t="n" s="25">
         <v>0.5</v>
@@ -2932,31 +2932,31 @@
         <v>69.0</v>
       </c>
       <c r="E69" t="n" s="25">
-        <v>0.8935715186844914</v>
+        <v>0.8779114581988025</v>
       </c>
       <c r="F69" t="n" s="25">
-        <v>0.32254993587399555</v>
+        <v>0.27477177564485866</v>
       </c>
       <c r="G69" t="n" s="25">
-        <v>0.042758532755608765</v>
+        <v>0.018887028220969375</v>
       </c>
       <c r="H69" t="n" s="25">
-        <v>0.16680047043535226</v>
+        <v>0.1424204533408533</v>
       </c>
       <c r="I69" t="n" s="25">
-        <v>1.3456034697495197E-5</v>
+        <v>5.448070020875329E-6</v>
       </c>
       <c r="J69" t="n" s="25">
-        <v>1.0500449759681099E-16</v>
+        <v>1.27947291196209E-17</v>
       </c>
       <c r="K69" t="n" s="25">
-        <v>1.860942535933047E-4</v>
+        <v>1.5227261631857678E-4</v>
       </c>
       <c r="L69" t="n" s="25">
-        <v>4.090846041656707E-18</v>
+        <v>1.6057746455121442E-18</v>
       </c>
       <c r="M69" t="n" s="25">
-        <v>8.547345227445463E-39</v>
+        <v>1.1638798178625559E-39</v>
       </c>
       <c r="N69" t="n" s="25">
         <v>0.5</v>
@@ -2967,31 +2967,31 @@
         <v>70.0</v>
       </c>
       <c r="E70" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F70" t="n" s="25">
-        <v>0.9846160912713838</v>
+        <v>0.9697226048646548</v>
       </c>
       <c r="G70" t="n" s="25">
-        <v>0.5163693392322637</v>
+        <v>0.36552750161596786</v>
       </c>
       <c r="H70" t="n" s="25">
-        <v>0.9962244703962657</v>
+        <v>0.9922117582024361</v>
       </c>
       <c r="I70" t="n" s="25">
-        <v>0.9821457502618601</v>
+        <v>0.9506580149604209</v>
       </c>
       <c r="J70" t="n" s="25">
-        <v>0.07263190390293803</v>
+        <v>0.004043234413595831</v>
       </c>
       <c r="K70" t="n" s="25">
-        <v>0.9332724783908215</v>
+        <v>0.8950131043499049</v>
       </c>
       <c r="L70" t="n" s="25">
-        <v>0.517453140359446</v>
+        <v>0.10220384445346818</v>
       </c>
       <c r="M70" t="n" s="25">
-        <v>6.162521522306197E-12</v>
+        <v>8.696348477281376E-14</v>
       </c>
       <c r="N70" t="n" s="25">
         <v>0.5</v>
@@ -3002,31 +3002,31 @@
         <v>71.0</v>
       </c>
       <c r="E71" t="n" s="25">
-        <v>0.05254178825544757</v>
+        <v>0.051307103553501335</v>
       </c>
       <c r="F71" t="n" s="25">
-        <v>0.0026839554637366845</v>
+        <v>0.002214968119455221</v>
       </c>
       <c r="G71" t="n" s="25">
-        <v>5.420040500755498E-5</v>
+        <v>3.347142131548756E-5</v>
       </c>
       <c r="H71" t="n" s="25">
-        <v>0.0010749384698689394</v>
+        <v>8.789874500987182E-4</v>
       </c>
       <c r="I71" t="n" s="25">
-        <v>2.974333763997543E-8</v>
+        <v>9.272082423500673E-9</v>
       </c>
       <c r="J71" t="n" s="25">
-        <v>8.841719128477957E-17</v>
+        <v>1.2484440605601984E-17</v>
       </c>
       <c r="K71" t="n" s="25">
-        <v>1.0442606495168851E-5</v>
+        <v>4.851061793311413E-6</v>
       </c>
       <c r="L71" t="n" s="25">
-        <v>5.2891249672249673E-14</v>
+        <v>1.779290683324116E-15</v>
       </c>
       <c r="M71" t="n" s="25">
-        <v>1.5940936498053334E-30</v>
+        <v>2.837376743491107E-32</v>
       </c>
       <c r="N71" t="n" s="25">
         <v>0.5</v>
@@ -3037,31 +3037,31 @@
         <v>72.0</v>
       </c>
       <c r="E72" t="n" s="25">
-        <v>0.9912258264167488</v>
+        <v>0.9891754785718329</v>
       </c>
       <c r="F72" t="n" s="25">
-        <v>0.7282367210905489</v>
+        <v>0.6583442845754087</v>
       </c>
       <c r="G72" t="n" s="25">
-        <v>0.49939421906980314</v>
+        <v>0.2511527401270782</v>
       </c>
       <c r="H72" t="n" s="25">
-        <v>0.7459872535742234</v>
+        <v>0.6932996268984821</v>
       </c>
       <c r="I72" t="n" s="25">
-        <v>0.43281967073350053</v>
+        <v>0.2201880439177796</v>
       </c>
       <c r="J72" t="n" s="25">
-        <v>0.3855220833760456</v>
+        <v>0.004067371688236353</v>
       </c>
       <c r="K72" t="n" s="25">
-        <v>0.34450424339953917</v>
+        <v>0.2800344151024188</v>
       </c>
       <c r="L72" t="n" s="25">
-        <v>1.4607074753450033E-4</v>
+        <v>2.6417835460638176E-5</v>
       </c>
       <c r="M72" t="n" s="25">
-        <v>1.4474875498188639E-11</v>
+        <v>8.64908620710228E-14</v>
       </c>
       <c r="N72" t="n" s="25">
         <v>0.5</v>
@@ -3072,31 +3072,31 @@
         <v>73.0</v>
       </c>
       <c r="E73" t="n" s="25">
-        <v>0.992947923756519</v>
+        <v>0.9910605253219646</v>
       </c>
       <c r="F73" t="n" s="25">
-        <v>0.7395608364564317</v>
+        <v>0.6692124532920855</v>
       </c>
       <c r="G73" t="n" s="25">
-        <v>0.08610297664762573</v>
+        <v>0.06211462194401815</v>
       </c>
       <c r="H73" t="n" s="25">
-        <v>0.7506051775997811</v>
+        <v>0.6897473585048206</v>
       </c>
       <c r="I73" t="n" s="25">
-        <v>0.6614857878238184</v>
+        <v>0.3858681254773458</v>
       </c>
       <c r="J73" t="n" s="25">
-        <v>7.577696032474243E-10</v>
+        <v>1.6719549197397192E-10</v>
       </c>
       <c r="K73" t="n" s="25">
-        <v>0.06037434559471889</v>
+        <v>0.0515359010160508</v>
       </c>
       <c r="L73" t="n" s="25">
-        <v>4.666525064966271E-9</v>
+        <v>1.3384016124198308E-9</v>
       </c>
       <c r="M73" t="n" s="25">
-        <v>2.7872106718791557E-31</v>
+        <v>5.525166452963585E-32</v>
       </c>
       <c r="N73" t="n" s="25">
         <v>0.5</v>
@@ -3107,31 +3107,31 @@
         <v>74.0</v>
       </c>
       <c r="E74" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F74" t="n" s="25">
-        <v>0.9999990823987623</v>
+        <v>0.9999955086148147</v>
       </c>
       <c r="G74" t="n" s="25">
-        <v>0.9999999999912884</v>
+        <v>0.9999999989250976</v>
       </c>
       <c r="H74" t="n" s="25">
-        <v>0.9997210606059247</v>
+        <v>0.9994065143196758</v>
       </c>
       <c r="I74" t="n" s="25">
-        <v>0.9999999999851495</v>
+        <v>0.9999999988706394</v>
       </c>
       <c r="J74" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999997207254</v>
       </c>
       <c r="K74" t="n" s="25">
-        <v>0.9971644721368537</v>
+        <v>0.9928089477688027</v>
       </c>
       <c r="L74" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9997356603233037</v>
       </c>
       <c r="M74" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9997201512118395</v>
       </c>
       <c r="N74" t="n" s="25">
         <v>0.5</v>
@@ -3142,31 +3142,31 @@
         <v>75.0</v>
       </c>
       <c r="E75" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F75" t="n" s="25">
-        <v>0.9999667352490874</v>
+        <v>0.9998879642380039</v>
       </c>
       <c r="G75" t="n" s="25">
-        <v>0.9999837845681634</v>
+        <v>0.9997812403119108</v>
       </c>
       <c r="H75" t="n" s="25">
-        <v>0.9999791814276808</v>
+        <v>0.9999300205156114</v>
       </c>
       <c r="I75" t="n" s="25">
-        <v>0.9999999990930494</v>
+        <v>0.9999999082799284</v>
       </c>
       <c r="J75" t="n" s="25">
-        <v>1.0</v>
+        <v>0.999982430786282</v>
       </c>
       <c r="K75" t="n" s="25">
-        <v>0.9999784084356614</v>
+        <v>0.9997592586938954</v>
       </c>
       <c r="L75" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999291702528025</v>
       </c>
       <c r="M75" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9855075865425781</v>
       </c>
       <c r="N75" t="n" s="25">
         <v>0.5</v>
@@ -3177,31 +3177,31 @@
         <v>76.0</v>
       </c>
       <c r="E76" t="n" s="25">
-        <v>0.9990914510156967</v>
+        <v>0.9988209996328056</v>
       </c>
       <c r="F76" t="n" s="25">
-        <v>0.995641169468445</v>
+        <v>0.9901879493181119</v>
       </c>
       <c r="G76" t="n" s="25">
-        <v>0.5839797293620315</v>
+        <v>0.4668075540311963</v>
       </c>
       <c r="H76" t="n" s="25">
-        <v>0.9989132036117151</v>
+        <v>0.9974645665356345</v>
       </c>
       <c r="I76" t="n" s="25">
-        <v>0.9960139305121508</v>
+        <v>0.9875028233746891</v>
       </c>
       <c r="J76" t="n" s="25">
-        <v>1.0</v>
+        <v>0.0013548660098977744</v>
       </c>
       <c r="K76" t="n" s="25">
-        <v>0.9404338394289937</v>
+        <v>0.9080188985913388</v>
       </c>
       <c r="L76" t="n" s="25">
-        <v>1.0</v>
+        <v>0.14593183023233572</v>
       </c>
       <c r="M76" t="n" s="25">
-        <v>1.0</v>
+        <v>2.890663143033468E-14</v>
       </c>
       <c r="N76" t="n" s="25">
         <v>0.5</v>
@@ -3212,31 +3212,31 @@
         <v>77.0</v>
       </c>
       <c r="E77" t="n" s="25">
-        <v>0.9914182166327893</v>
+        <v>0.9893826423696792</v>
       </c>
       <c r="F77" t="n" s="25">
-        <v>0.6772006570992029</v>
+        <v>0.6207681004887406</v>
       </c>
       <c r="G77" t="n" s="25">
-        <v>0.014826302082568273</v>
+        <v>0.01027451217555848</v>
       </c>
       <c r="H77" t="n" s="25">
-        <v>0.6373978071908569</v>
+        <v>0.5952653608760213</v>
       </c>
       <c r="I77" t="n" s="25">
-        <v>0.07008976353459186</v>
+        <v>0.03058036220648944</v>
       </c>
       <c r="J77" t="n" s="25">
-        <v>9.428231278206803E-14</v>
+        <v>2.6328696601467456E-14</v>
       </c>
       <c r="K77" t="n" s="25">
-        <v>0.08236000504166623</v>
+        <v>0.07305953136385215</v>
       </c>
       <c r="L77" t="n" s="25">
-        <v>8.384723156347145E-11</v>
+        <v>3.179157548369678E-11</v>
       </c>
       <c r="M77" t="n" s="25">
-        <v>8.331608075235104E-36</v>
+        <v>2.2610506083042857E-36</v>
       </c>
       <c r="N77" t="n" s="25">
         <v>0.5</v>
@@ -3247,31 +3247,31 @@
         <v>78.0</v>
       </c>
       <c r="E78" t="n" s="25">
-        <v>0.9987908017528341</v>
+        <v>0.9984807825459784</v>
       </c>
       <c r="F78" t="n" s="25">
-        <v>0.9999310580742411</v>
+        <v>0.9997624795227325</v>
       </c>
       <c r="G78" t="n" s="25">
-        <v>0.9995741726743654</v>
+        <v>0.9976638621285688</v>
       </c>
       <c r="H78" t="n" s="25">
-        <v>0.9964821574623373</v>
+        <v>0.9940703782231741</v>
       </c>
       <c r="I78" t="n" s="25">
-        <v>0.9940098293284516</v>
+        <v>0.9837427759675492</v>
       </c>
       <c r="J78" t="n" s="25">
-        <v>0.9931364064162888</v>
+        <v>0.8869897838688786</v>
       </c>
       <c r="K78" t="n" s="25">
-        <v>0.6571193609828055</v>
+        <v>0.6281591015517493</v>
       </c>
       <c r="L78" t="n" s="25">
-        <v>0.28514324681731956</v>
+        <v>0.179182523127571</v>
       </c>
       <c r="M78" t="n" s="25">
-        <v>9.898593922618603E-8</v>
+        <v>3.3891942377314222E-9</v>
       </c>
       <c r="N78" t="n" s="25">
         <v>0.5</v>
@@ -3282,31 +3282,31 @@
         <v>79.0</v>
       </c>
       <c r="E79" t="n" s="25">
-        <v>0.9992196587541278</v>
+        <v>0.9989685783821551</v>
       </c>
       <c r="F79" t="n" s="25">
-        <v>0.9993135697059193</v>
+        <v>0.9978098114809945</v>
       </c>
       <c r="G79" t="n" s="25">
-        <v>0.99779081398428</v>
+        <v>0.9800618364520084</v>
       </c>
       <c r="H79" t="n" s="25">
-        <v>0.9974146947028855</v>
+        <v>0.994247065324608</v>
       </c>
       <c r="I79" t="n" s="25">
-        <v>0.9994023257335464</v>
+        <v>0.9938795706381632</v>
       </c>
       <c r="J79" t="n" s="25">
-        <v>0.9999167407936359</v>
+        <v>0.994073436822224</v>
       </c>
       <c r="K79" t="n" s="25">
-        <v>0.6010716190568155</v>
+        <v>0.5596487307237161</v>
       </c>
       <c r="L79" t="n" s="25">
-        <v>0.031813638812786024</v>
+        <v>0.012439771509323502</v>
       </c>
       <c r="M79" t="n" s="25">
-        <v>3.1545499810051316E-8</v>
+        <v>6.011195239903294E-10</v>
       </c>
       <c r="N79" t="n" s="25">
         <v>0.5</v>
@@ -3317,31 +3317,31 @@
         <v>80.0</v>
       </c>
       <c r="E80" t="n" s="25">
-        <v>0.9947553421113411</v>
+        <v>0.9933874210505322</v>
       </c>
       <c r="F80" t="n" s="25">
-        <v>0.9172653235135276</v>
+        <v>0.8608434316129117</v>
       </c>
       <c r="G80" t="n" s="25">
-        <v>0.14481490618952508</v>
+        <v>0.10766185061995134</v>
       </c>
       <c r="H80" t="n" s="25">
-        <v>0.960948364686511</v>
+        <v>0.9290925758714884</v>
       </c>
       <c r="I80" t="n" s="25">
-        <v>0.9659353700671779</v>
+        <v>0.8996973170568787</v>
       </c>
       <c r="J80" t="n" s="25">
-        <v>5.655582402084337E-6</v>
+        <v>9.289302814402586E-7</v>
       </c>
       <c r="K80" t="n" s="25">
-        <v>0.6097912058113175</v>
+        <v>0.5272038157281751</v>
       </c>
       <c r="L80" t="n" s="25">
-        <v>0.0010150917874914105</v>
+        <v>1.6719771948005998E-4</v>
       </c>
       <c r="M80" t="n" s="25">
-        <v>1.3356994519943323E-21</v>
+        <v>9.225115731221716E-23</v>
       </c>
       <c r="N80" t="n" s="25">
         <v>0.5</v>
@@ -3352,31 +3352,31 @@
         <v>81.0</v>
       </c>
       <c r="E81" t="n" s="25">
-        <v>0.05214053541956365</v>
+        <v>0.05098591985439762</v>
       </c>
       <c r="F81" t="n" s="25">
-        <v>0.002198159349036692</v>
+        <v>0.00185554122116827</v>
       </c>
       <c r="G81" t="n" s="25">
-        <v>3.9330294256679073E-4</v>
+        <v>1.3510079645135298E-4</v>
       </c>
       <c r="H81" t="n" s="25">
-        <v>8.911976386671951E-4</v>
+        <v>7.452447713942668E-4</v>
       </c>
       <c r="I81" t="n" s="25">
-        <v>2.7972836147345642E-8</v>
+        <v>1.0454776124379936E-8</v>
       </c>
       <c r="J81" t="n" s="25">
-        <v>1.0</v>
+        <v>1.162732989238614E-11</v>
       </c>
       <c r="K81" t="n" s="25">
-        <v>1.6304922111732804E-5</v>
+        <v>9.312738120870887E-6</v>
       </c>
       <c r="L81" t="n" s="25">
-        <v>1.0</v>
+        <v>8.851677622483617E-15</v>
       </c>
       <c r="M81" t="n" s="25">
-        <v>1.0</v>
+        <v>4.1066129800326255E-23</v>
       </c>
       <c r="N81" t="n" s="25">
         <v>0.5</v>
@@ -3387,31 +3387,31 @@
         <v>82.0</v>
       </c>
       <c r="E82" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F82" t="n" s="25">
-        <v>0.9830944309164982</v>
+        <v>0.9676652819140397</v>
       </c>
       <c r="G82" t="n" s="25">
-        <v>0.32931596525471374</v>
+        <v>0.23450775175412095</v>
       </c>
       <c r="H82" t="n" s="25">
-        <v>0.9917169487612278</v>
+        <v>0.9850445633666501</v>
       </c>
       <c r="I82" t="n" s="25">
-        <v>0.981511626289819</v>
+        <v>0.9499912533322348</v>
       </c>
       <c r="J82" t="n" s="25">
-        <v>1.7980260577709427E-4</v>
+        <v>1.938569786258422E-5</v>
       </c>
       <c r="K82" t="n" s="25">
-        <v>0.6971358491027009</v>
+        <v>0.6697020403845751</v>
       </c>
       <c r="L82" t="n" s="25">
-        <v>6.071500387232117E-4</v>
+        <v>2.398585974712319E-4</v>
       </c>
       <c r="M82" t="n" s="25">
-        <v>1.787284620535408E-20</v>
+        <v>1.6969300723836505E-21</v>
       </c>
       <c r="N82" t="n" s="25">
         <v>0.5</v>
@@ -3422,31 +3422,31 @@
         <v>83.0</v>
       </c>
       <c r="E83" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F83" t="n" s="25">
-        <v>0.9819609413641635</v>
+        <v>0.9660997502721836</v>
       </c>
       <c r="G83" t="n" s="25">
-        <v>0.18177945350846686</v>
+        <v>0.1360132560042527</v>
       </c>
       <c r="H83" t="n" s="25">
-        <v>0.9917169487612278</v>
+        <v>0.9850445633666501</v>
       </c>
       <c r="I83" t="n" s="25">
-        <v>0.9815082250157697</v>
+        <v>0.9499857398595162</v>
       </c>
       <c r="J83" t="n" s="25">
-        <v>2.501425504305147E-6</v>
+        <v>4.701410554689514E-7</v>
       </c>
       <c r="K83" t="n" s="25">
-        <v>0.6971051531045412</v>
+        <v>0.6696803375782686</v>
       </c>
       <c r="L83" t="n" s="25">
-        <v>1.5185665951317057E-4</v>
+        <v>5.997543858621399E-5</v>
       </c>
       <c r="M83" t="n" s="25">
-        <v>3.297816175103146E-24</v>
+        <v>5.0252523865497E-25</v>
       </c>
       <c r="N83" t="n" s="25">
         <v>0.5</v>
@@ -3457,31 +3457,31 @@
         <v>84.0</v>
       </c>
       <c r="E84" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F84" t="n" s="25">
-        <v>0.9999988977970082</v>
+        <v>0.9999949099649094</v>
       </c>
       <c r="G84" t="n" s="25">
-        <v>0.9999999980441813</v>
+        <v>0.9999998842667239</v>
       </c>
       <c r="H84" t="n" s="25">
-        <v>0.9999895566146154</v>
+        <v>0.9999655494025596</v>
       </c>
       <c r="I84" t="n" s="25">
-        <v>0.999999999993433</v>
+        <v>0.999999998816382</v>
       </c>
       <c r="J84" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999978078828</v>
       </c>
       <c r="K84" t="n" s="25">
-        <v>0.9991629048588412</v>
+        <v>0.995778769845021</v>
       </c>
       <c r="L84" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9998643576628202</v>
       </c>
       <c r="M84" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9997459390599722</v>
       </c>
       <c r="N84" t="n" s="25">
         <v>0.5</v>
@@ -3492,31 +3492,31 @@
         <v>85.0</v>
       </c>
       <c r="E85" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F85" t="n" s="25">
-        <v>0.9999990823987623</v>
+        <v>0.9999955086148147</v>
       </c>
       <c r="G85" t="n" s="25">
-        <v>0.9999999999912884</v>
+        <v>0.9999999989250976</v>
       </c>
       <c r="H85" t="n" s="25">
-        <v>0.9998142743894936</v>
+        <v>0.999577198045728</v>
       </c>
       <c r="I85" t="n" s="25">
-        <v>0.9999999999961092</v>
+        <v>0.9999999996152397</v>
       </c>
       <c r="J85" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999999908123</v>
       </c>
       <c r="K85" t="n" s="25">
-        <v>0.9996931334938806</v>
+        <v>0.9987903785670498</v>
       </c>
       <c r="L85" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999986530649053</v>
       </c>
       <c r="M85" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999942482729668</v>
       </c>
       <c r="N85" t="n" s="25">
         <v>0.5</v>
@@ -3527,31 +3527,31 @@
         <v>86.0</v>
       </c>
       <c r="E86" t="n" s="25">
-        <v>0.9991756368707945</v>
+        <v>0.998918239907052</v>
       </c>
       <c r="F86" t="n" s="25">
-        <v>0.9999789210182987</v>
+        <v>0.9999226627331868</v>
       </c>
       <c r="G86" t="n" s="25">
-        <v>0.9999992478379878</v>
+        <v>0.9999808335863607</v>
       </c>
       <c r="H86" t="n" s="25">
-        <v>0.9998495167292063</v>
+        <v>0.9996234844125298</v>
       </c>
       <c r="I86" t="n" s="25">
-        <v>0.9999999662025593</v>
+        <v>0.9999984493128541</v>
       </c>
       <c r="J86" t="n" s="25">
-        <v>0.99999996843312</v>
+        <v>0.9999965671095054</v>
       </c>
       <c r="K86" t="n" s="25">
-        <v>0.9773538275123429</v>
+        <v>0.9459591161731286</v>
       </c>
       <c r="L86" t="n" s="25">
-        <v>0.9930467019228778</v>
+        <v>0.9674879903131516</v>
       </c>
       <c r="M86" t="n" s="25">
-        <v>0.5509988110141046</v>
+        <v>0.03543393802257903</v>
       </c>
       <c r="N86" t="n" s="25">
         <v>0.5</v>
@@ -3562,31 +3562,31 @@
         <v>87.0</v>
       </c>
       <c r="E87" t="n" s="25">
-        <v>0.9988995972197205</v>
+        <v>0.9986027661696405</v>
       </c>
       <c r="F87" t="n" s="25">
-        <v>0.9999844453618442</v>
+        <v>0.9999336358554359</v>
       </c>
       <c r="G87" t="n" s="25">
-        <v>0.9999999939840335</v>
+        <v>0.9999995483201389</v>
       </c>
       <c r="H87" t="n" s="25">
-        <v>0.9987038934517164</v>
+        <v>0.9974782637062687</v>
       </c>
       <c r="I87" t="n" s="25">
-        <v>0.999999957904069</v>
+        <v>0.9999980937771281</v>
       </c>
       <c r="J87" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999994610058324</v>
       </c>
       <c r="K87" t="n" s="25">
-        <v>0.981332136792971</v>
+        <v>0.9586288659822149</v>
       </c>
       <c r="L87" t="n" s="25">
-        <v>1.0</v>
+        <v>0.976647527611322</v>
       </c>
       <c r="M87" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9482949717324879</v>
       </c>
       <c r="N87" t="n" s="25">
         <v>0.5</v>
@@ -3597,31 +3597,31 @@
         <v>88.0</v>
       </c>
       <c r="E88" t="n" s="25">
-        <v>0.012338572020197454</v>
+        <v>0.012152239495593305</v>
       </c>
       <c r="F88" t="n" s="25">
-        <v>4.579065480111406E-5</v>
+        <v>3.8830213462692176E-5</v>
       </c>
       <c r="G88" t="n" s="25">
-        <v>1.7454582610165527E-6</v>
+        <v>6.3684583386375E-7</v>
       </c>
       <c r="H88" t="n" s="25">
-        <v>3.5072227440104204E-5</v>
+        <v>2.940442305819729E-5</v>
       </c>
       <c r="I88" t="n" s="25">
-        <v>2.913655581803462E-11</v>
+        <v>9.888314095816727E-12</v>
       </c>
       <c r="J88" t="n" s="25">
-        <v>6.999083205163413E-13</v>
+        <v>4.491707274419936E-15</v>
       </c>
       <c r="K88" t="n" s="25">
-        <v>1.5500969744223087E-8</v>
+        <v>1.2777881462703959E-8</v>
       </c>
       <c r="L88" t="n" s="25">
-        <v>9.527767547494424E-20</v>
+        <v>3.213152726383689E-20</v>
       </c>
       <c r="M88" t="n" s="25">
-        <v>2.4977352114538565E-28</v>
+        <v>2.7082767043440872E-30</v>
       </c>
       <c r="N88" t="n" s="25">
         <v>0.5</v>
@@ -3632,31 +3632,31 @@
         <v>89.0</v>
       </c>
       <c r="E89" t="n" s="25">
-        <v>0.9991756368707945</v>
+        <v>0.998918239907052</v>
       </c>
       <c r="F89" t="n" s="25">
-        <v>0.9994326374676378</v>
+        <v>0.9981581814595369</v>
       </c>
       <c r="G89" t="n" s="25">
-        <v>0.9999720664049687</v>
+        <v>0.9993493132189577</v>
       </c>
       <c r="H89" t="n" s="25">
-        <v>0.9980253053398608</v>
+        <v>0.9952315046379036</v>
       </c>
       <c r="I89" t="n" s="25">
-        <v>0.999992297268676</v>
+        <v>0.9996930648774699</v>
       </c>
       <c r="J89" t="n" s="25">
-        <v>0.9999994058202447</v>
+        <v>0.999923988842448</v>
       </c>
       <c r="K89" t="n" s="25">
-        <v>0.9631750441707343</v>
+        <v>0.8982406362899054</v>
       </c>
       <c r="L89" t="n" s="25">
-        <v>0.9915464392797556</v>
+        <v>0.919210509235624</v>
       </c>
       <c r="M89" t="n" s="25">
-        <v>0.5755918530458941</v>
+        <v>0.01822647664811671</v>
       </c>
       <c r="N89" t="n" s="25">
         <v>0.5</v>
@@ -3667,31 +3667,31 @@
         <v>90.0</v>
       </c>
       <c r="E90" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F90" t="n" s="25">
-        <v>0.9999952660458776</v>
+        <v>0.999982693245053</v>
       </c>
       <c r="G90" t="n" s="25">
-        <v>0.9999950253225662</v>
+        <v>0.9999280496953432</v>
       </c>
       <c r="H90" t="n" s="25">
-        <v>0.9999891381890671</v>
+        <v>0.9999645709177181</v>
       </c>
       <c r="I90" t="n" s="25">
-        <v>0.9999999969883095</v>
+        <v>0.9999997899631679</v>
       </c>
       <c r="J90" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999889090002706</v>
       </c>
       <c r="K90" t="n" s="25">
-        <v>0.9975477958779256</v>
+        <v>0.989275721491841</v>
       </c>
       <c r="L90" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9957910123006065</v>
       </c>
       <c r="M90" t="n" s="25">
-        <v>1.0</v>
+        <v>0.37675026176036086</v>
       </c>
       <c r="N90" t="n" s="25">
         <v>0.5</v>
@@ -3702,31 +3702,31 @@
         <v>91.0</v>
       </c>
       <c r="E91" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F91" t="n" s="25">
-        <v>0.9590076589019396</v>
+        <v>0.9329745903762626</v>
       </c>
       <c r="G91" t="n" s="25">
-        <v>0.3303377140800883</v>
+        <v>0.23013758946820348</v>
       </c>
       <c r="H91" t="n" s="25">
-        <v>0.9607503279843453</v>
+        <v>0.9407221809024124</v>
       </c>
       <c r="I91" t="n" s="25">
-        <v>0.9117008653741715</v>
+        <v>0.80207125034312</v>
       </c>
       <c r="J91" t="n" s="25">
-        <v>7.495998073836504E-7</v>
+        <v>1.1327052992641025E-7</v>
       </c>
       <c r="K91" t="n" s="25">
-        <v>0.47931801140630714</v>
+        <v>0.4477973182009264</v>
       </c>
       <c r="L91" t="n" s="25">
-        <v>8.933885508776806E-6</v>
+        <v>3.338886451287276E-6</v>
       </c>
       <c r="M91" t="n" s="25">
-        <v>3.576700517137557E-25</v>
+        <v>5.16288659249545E-26</v>
       </c>
       <c r="N91" t="n" s="25">
         <v>0.5</v>
@@ -3737,31 +3737,31 @@
         <v>92.0</v>
       </c>
       <c r="E92" t="n" s="25">
-        <v>0.9919646742851658</v>
+        <v>0.9899828039505366</v>
       </c>
       <c r="F92" t="n" s="25">
-        <v>0.9986818159606842</v>
+        <v>0.995067174794749</v>
       </c>
       <c r="G92" t="n" s="25">
-        <v>0.9999995819811105</v>
+        <v>0.999974092732867</v>
       </c>
       <c r="H92" t="n" s="25">
-        <v>0.9638766177730557</v>
+        <v>0.9344401497902913</v>
       </c>
       <c r="I92" t="n" s="25">
-        <v>0.9999889868627162</v>
+        <v>0.9996462331372682</v>
       </c>
       <c r="J92" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999935675333524</v>
       </c>
       <c r="K92" t="n" s="25">
-        <v>0.43194112202482676</v>
+        <v>0.33597319759519445</v>
       </c>
       <c r="L92" t="n" s="25">
-        <v>1.0</v>
+        <v>0.14896859658929212</v>
       </c>
       <c r="M92" t="n" s="25">
-        <v>1.0</v>
+        <v>0.010316421622395424</v>
       </c>
       <c r="N92" t="n" s="25">
         <v>0.5</v>
@@ -3772,31 +3772,31 @@
         <v>93.0</v>
       </c>
       <c r="E93" t="n" s="25">
-        <v>0.9992923581596833</v>
+        <v>0.9990541090525831</v>
       </c>
       <c r="F93" t="n" s="25">
-        <v>0.9997929366027748</v>
+        <v>0.9993774508979147</v>
       </c>
       <c r="G93" t="n" s="25">
-        <v>0.9598963197181126</v>
+        <v>0.9243344804784598</v>
       </c>
       <c r="H93" t="n" s="25">
-        <v>0.999398760622715</v>
+        <v>0.9985046703947374</v>
       </c>
       <c r="I93" t="n" s="25">
-        <v>0.9994045548928713</v>
+        <v>0.9977758811387046</v>
       </c>
       <c r="J93" t="n" s="25">
-        <v>0.5903993478591412</v>
+        <v>0.13221614252453376</v>
       </c>
       <c r="K93" t="n" s="25">
-        <v>0.6168396709052179</v>
+        <v>0.5713540818563041</v>
       </c>
       <c r="L93" t="n" s="25">
-        <v>0.010553231455536854</v>
+        <v>0.004035081808184899</v>
       </c>
       <c r="M93" t="n" s="25">
-        <v>1.4710913306303217E-14</v>
+        <v>7.980706611804874E-16</v>
       </c>
       <c r="N93" t="n" s="25">
         <v>0.5</v>
@@ -3807,31 +3807,31 @@
         <v>94.0</v>
       </c>
       <c r="E94" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F94" t="n" s="25">
-        <v>0.9999990823987623</v>
+        <v>0.9999955086148147</v>
       </c>
       <c r="G94" t="n" s="25">
-        <v>0.9999999999912884</v>
+        <v>0.9999999989250976</v>
       </c>
       <c r="H94" t="n" s="25">
-        <v>0.9997210606059247</v>
+        <v>0.9994065143196758</v>
       </c>
       <c r="I94" t="n" s="25">
-        <v>0.9999999999851495</v>
+        <v>0.9999999988706394</v>
       </c>
       <c r="J94" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999997207254</v>
       </c>
       <c r="K94" t="n" s="25">
-        <v>0.9971644721368537</v>
+        <v>0.9928089477688027</v>
       </c>
       <c r="L94" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9997356603233037</v>
       </c>
       <c r="M94" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9997201512118395</v>
       </c>
       <c r="N94" t="n" s="25">
         <v>0.5</v>
@@ -3842,31 +3842,31 @@
         <v>95.0</v>
       </c>
       <c r="E95" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F95" t="n" s="25">
-        <v>0.9996703233435946</v>
+        <v>0.9990886588762357</v>
       </c>
       <c r="G95" t="n" s="25">
-        <v>0.9201948765167828</v>
+        <v>0.8746684222698341</v>
       </c>
       <c r="H95" t="n" s="25">
-        <v>0.9995863747398582</v>
+        <v>0.9988684295382624</v>
       </c>
       <c r="I95" t="n" s="25">
-        <v>0.9992092768854614</v>
+        <v>0.9970839976932451</v>
       </c>
       <c r="J95" t="n" s="25">
-        <v>0.09323313893492295</v>
+        <v>0.017732899783322</v>
       </c>
       <c r="K95" t="n" s="25">
-        <v>0.9075629974169231</v>
+        <v>0.8481148139556499</v>
       </c>
       <c r="L95" t="n" s="25">
-        <v>0.7824206871393226</v>
+        <v>0.262186069838377</v>
       </c>
       <c r="M95" t="n" s="25">
-        <v>2.01439470226036E-12</v>
+        <v>4.680725142966741E-14</v>
       </c>
       <c r="N95" t="n" s="25">
         <v>0.5</v>
@@ -3877,31 +3877,31 @@
         <v>96.0</v>
       </c>
       <c r="E96" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F96" t="n" s="25">
-        <v>0.9999181594871551</v>
+        <v>0.9996939558218835</v>
       </c>
       <c r="G96" t="n" s="25">
-        <v>0.9999933627923566</v>
+        <v>0.9998279088856284</v>
       </c>
       <c r="H96" t="n" s="25">
-        <v>0.9843752713654105</v>
+        <v>0.9672318851400753</v>
       </c>
       <c r="I96" t="n" s="25">
-        <v>0.9989789710216792</v>
+        <v>0.9806295038664927</v>
       </c>
       <c r="J96" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9976191737311834</v>
       </c>
       <c r="K96" t="n" s="25">
-        <v>0.7478019115959231</v>
+        <v>0.5308533088659005</v>
       </c>
       <c r="L96" t="n" s="25">
-        <v>1.0</v>
+        <v>0.27145163648758797</v>
       </c>
       <c r="M96" t="n" s="25">
-        <v>1.0</v>
+        <v>0.05306845499520527</v>
       </c>
       <c r="N96" t="n" s="25">
         <v>0.5</v>
@@ -3912,31 +3912,31 @@
         <v>97.0</v>
       </c>
       <c r="E97" t="n" s="25">
-        <v>0.9987908017528341</v>
+        <v>0.9984807825459784</v>
       </c>
       <c r="F97" t="n" s="25">
-        <v>0.9999980651573475</v>
+        <v>0.9999913887212901</v>
       </c>
       <c r="G97" t="n" s="25">
-        <v>0.9999999992271364</v>
+        <v>0.9999999410373535</v>
       </c>
       <c r="H97" t="n" s="25">
-        <v>0.9989643609729629</v>
+        <v>0.9981392213905914</v>
       </c>
       <c r="I97" t="n" s="25">
-        <v>0.9999999874895829</v>
+        <v>0.999999585608274</v>
       </c>
       <c r="J97" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999995008804542</v>
       </c>
       <c r="K97" t="n" s="25">
-        <v>0.9917413568970627</v>
+        <v>0.9826668191907068</v>
       </c>
       <c r="L97" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9937493567507688</v>
       </c>
       <c r="M97" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9861665401394457</v>
       </c>
       <c r="N97" t="n" s="25">
         <v>0.5</v>
@@ -3947,31 +3947,31 @@
         <v>98.0</v>
       </c>
       <c r="E98" t="n" s="25">
-        <v>0.9993584866597034</v>
+        <v>0.9991327925756758</v>
       </c>
       <c r="F98" t="n" s="25">
-        <v>0.9998784599643596</v>
+        <v>0.9995947685211373</v>
       </c>
       <c r="G98" t="n" s="25">
-        <v>0.9975279970867735</v>
+        <v>0.9931017663992115</v>
       </c>
       <c r="H98" t="n" s="25">
-        <v>0.9963652655073699</v>
+        <v>0.9913382617740153</v>
       </c>
       <c r="I98" t="n" s="25">
-        <v>0.9970176970103094</v>
+        <v>0.9896373512585626</v>
       </c>
       <c r="J98" t="n" s="25">
-        <v>0.8697004692943705</v>
+        <v>0.36394916793037</v>
       </c>
       <c r="K98" t="n" s="25">
-        <v>0.46004193116595027</v>
+        <v>0.3667324837696091</v>
       </c>
       <c r="L98" t="n" s="25">
-        <v>0.026198743081584618</v>
+        <v>0.0045667960261370115</v>
       </c>
       <c r="M98" t="n" s="25">
-        <v>2.90604489871873E-11</v>
+        <v>6.400046653138051E-13</v>
       </c>
       <c r="N98" t="n" s="25">
         <v>0.5</v>
@@ -3982,31 +3982,31 @@
         <v>99.0</v>
       </c>
       <c r="E99" t="n" s="25">
-        <v>0.9990023869597789</v>
+        <v>0.9987186878639994</v>
       </c>
       <c r="F99" t="n" s="25">
-        <v>0.9999904174188717</v>
+        <v>0.9999594469051148</v>
       </c>
       <c r="G99" t="n" s="25">
-        <v>0.9999990596735967</v>
+        <v>0.9999622806405726</v>
       </c>
       <c r="H99" t="n" s="25">
-        <v>0.9975165457185352</v>
+        <v>0.9947638966518697</v>
       </c>
       <c r="I99" t="n" s="25">
-        <v>0.9999532139746432</v>
+        <v>0.9987337007290777</v>
       </c>
       <c r="J99" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9995698499459309</v>
       </c>
       <c r="K99" t="n" s="25">
-        <v>0.9356017840184828</v>
+        <v>0.8398154263529871</v>
       </c>
       <c r="L99" t="n" s="25">
-        <v>1.0</v>
+        <v>0.8955635425805797</v>
       </c>
       <c r="M99" t="n" s="25">
-        <v>1.0</v>
+        <v>0.35665317154717757</v>
       </c>
       <c r="N99" t="n" s="25">
         <v>0.5</v>
@@ -4017,31 +4017,31 @@
         <v>100.0</v>
       </c>
       <c r="E100" t="n" s="25">
-        <v>0.9638411357973466</v>
+        <v>0.9567581524074854</v>
       </c>
       <c r="F100" t="n" s="25">
-        <v>0.4840362905832256</v>
+        <v>0.4275105751652396</v>
       </c>
       <c r="G100" t="n" s="25">
-        <v>0.04397689122527863</v>
+        <v>0.0262505787087478</v>
       </c>
       <c r="H100" t="n" s="25">
-        <v>0.3908975099673956</v>
+        <v>0.3447045634144185</v>
       </c>
       <c r="I100" t="n" s="25">
-        <v>0.03383766549583942</v>
+        <v>0.01298382746470873</v>
       </c>
       <c r="J100" t="n" s="25">
-        <v>7.226803666143031E-11</v>
+        <v>1.0904475104203305E-11</v>
       </c>
       <c r="K100" t="n" s="25">
-        <v>0.045063096145215004</v>
+        <v>0.032334063824594084</v>
       </c>
       <c r="L100" t="n" s="25">
-        <v>2.020658391414229E-9</v>
+        <v>3.5318551120029294E-10</v>
       </c>
       <c r="M100" t="n" s="25">
-        <v>6.218341590218176E-29</v>
+        <v>5.129212869965435E-30</v>
       </c>
       <c r="N100" t="n" s="25">
         <v>0.5</v>
@@ -4052,31 +4052,31 @@
         <v>101.0</v>
       </c>
       <c r="E101" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F101" t="n" s="25">
-        <v>0.9999769638830568</v>
+        <v>0.9999177842550951</v>
       </c>
       <c r="G101" t="n" s="25">
-        <v>0.999999540157244</v>
+        <v>0.9999904175560466</v>
       </c>
       <c r="H101" t="n" s="25">
-        <v>0.9999689506090006</v>
+        <v>0.9999016235253874</v>
       </c>
       <c r="I101" t="n" s="25">
-        <v>0.9999999999111292</v>
+        <v>0.9999999903047949</v>
       </c>
       <c r="J101" t="n" s="25">
-        <v>0.9999999953823512</v>
+        <v>0.9999992332831183</v>
       </c>
       <c r="K101" t="n" s="25">
-        <v>0.999918845286931</v>
+        <v>0.9993746905600268</v>
       </c>
       <c r="L101" t="n" s="25">
-        <v>0.9999926651801796</v>
+        <v>0.9997784248841499</v>
       </c>
       <c r="M101" t="n" s="25">
-        <v>0.9989299833739479</v>
+        <v>0.9484219585825963</v>
       </c>
       <c r="N101" t="n" s="25">
         <v>0.5</v>
@@ -4087,31 +4087,31 @@
         <v>102.0</v>
       </c>
       <c r="E102" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F102" t="n" s="25">
-        <v>0.9830944309164982</v>
+        <v>0.9676652819140397</v>
       </c>
       <c r="G102" t="n" s="25">
-        <v>0.3293307487755506</v>
+        <v>0.23451294513842832</v>
       </c>
       <c r="H102" t="n" s="25">
-        <v>0.9943397705692603</v>
+        <v>0.9891000947219253</v>
       </c>
       <c r="I102" t="n" s="25">
-        <v>0.981539472181201</v>
+        <v>0.950027747285985</v>
       </c>
       <c r="J102" t="n" s="25">
-        <v>4.4938531347595077E-4</v>
+        <v>4.846283542798054E-5</v>
       </c>
       <c r="K102" t="n" s="25">
-        <v>0.8483646209268596</v>
+        <v>0.8052329837725312</v>
       </c>
       <c r="L102" t="n" s="25">
-        <v>0.017236260656555882</v>
+        <v>0.0035568248691412343</v>
       </c>
       <c r="M102" t="n" s="25">
-        <v>1.1519350049034942E-17</v>
+        <v>5.667070605156182E-19</v>
       </c>
       <c r="N102" t="n" s="25">
         <v>0.5</v>
@@ -4122,31 +4122,31 @@
         <v>103.0</v>
       </c>
       <c r="E103" t="n" s="25">
-        <v>0.9990914510156967</v>
+        <v>0.9988209996328056</v>
       </c>
       <c r="F103" t="n" s="25">
-        <v>0.9949908012593469</v>
+        <v>0.9890836264015436</v>
       </c>
       <c r="G103" t="n" s="25">
-        <v>0.388291433049687</v>
+        <v>0.3102447946770831</v>
       </c>
       <c r="H103" t="n" s="25">
-        <v>0.9977595412036815</v>
+        <v>0.9953322950238781</v>
       </c>
       <c r="I103" t="n" s="25">
-        <v>0.9959307268858958</v>
+        <v>0.9873963875917345</v>
       </c>
       <c r="J103" t="n" s="25">
-        <v>8.638001093175546E-5</v>
+        <v>1.682862958908115E-5</v>
       </c>
       <c r="K103" t="n" s="25">
-        <v>0.7362998529179454</v>
+        <v>0.7065705352145046</v>
       </c>
       <c r="L103" t="n" s="25">
-        <v>0.0011323518763805712</v>
+        <v>4.5220941100728335E-4</v>
       </c>
       <c r="M103" t="n" s="25">
-        <v>9.7398471726486E-22</v>
+        <v>1.2448361525241365E-22</v>
       </c>
       <c r="N103" t="n" s="25">
         <v>0.5</v>
@@ -4157,31 +4157,31 @@
         <v>104.0</v>
       </c>
       <c r="E104" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F104" t="n" s="25">
-        <v>0.9830944309164982</v>
+        <v>0.9676652819140397</v>
       </c>
       <c r="G104" t="n" s="25">
-        <v>0.32931596525471374</v>
+        <v>0.23450775175412095</v>
       </c>
       <c r="H104" t="n" s="25">
-        <v>0.9917169487612278</v>
+        <v>0.9850445633666501</v>
       </c>
       <c r="I104" t="n" s="25">
-        <v>0.981511626289819</v>
+        <v>0.9499912533322348</v>
       </c>
       <c r="J104" t="n" s="25">
-        <v>1.7980260577709427E-4</v>
+        <v>1.938569786258422E-5</v>
       </c>
       <c r="K104" t="n" s="25">
-        <v>0.6971358491027009</v>
+        <v>0.6697020403845751</v>
       </c>
       <c r="L104" t="n" s="25">
-        <v>6.071500387232117E-4</v>
+        <v>2.398585974712319E-4</v>
       </c>
       <c r="M104" t="n" s="25">
-        <v>1.787284620535408E-20</v>
+        <v>1.6969300723836505E-21</v>
       </c>
       <c r="N104" t="n" s="25">
         <v>0.5</v>
@@ -4192,31 +4192,31 @@
         <v>105.0</v>
       </c>
       <c r="E105" t="n" s="25">
-        <v>0.9992923581596833</v>
+        <v>0.9990541090525831</v>
       </c>
       <c r="F105" t="n" s="25">
-        <v>0.9992230506224166</v>
+        <v>0.9976622214604911</v>
       </c>
       <c r="G105" t="n" s="25">
-        <v>0.9930935889153313</v>
+        <v>0.9805764546966158</v>
       </c>
       <c r="H105" t="n" s="25">
-        <v>0.9877821788050906</v>
+        <v>0.9755838995030277</v>
       </c>
       <c r="I105" t="n" s="25">
-        <v>0.9883518970255534</v>
+        <v>0.9657533083928772</v>
       </c>
       <c r="J105" t="n" s="25">
-        <v>0.23838697604994963</v>
+        <v>0.02455920663746876</v>
       </c>
       <c r="K105" t="n" s="25">
-        <v>0.2612436967838687</v>
+        <v>0.2265898765379453</v>
       </c>
       <c r="L105" t="n" s="25">
-        <v>1.5458056823051367E-4</v>
+        <v>5.4296017520842E-5</v>
       </c>
       <c r="M105" t="n" s="25">
-        <v>1.960422652839263E-16</v>
+        <v>9.909016688541381E-18</v>
       </c>
       <c r="N105" t="n" s="25">
         <v>0.5</v>
@@ -4227,31 +4227,31 @@
         <v>106.0</v>
       </c>
       <c r="E106" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F106" t="n" s="25">
-        <v>0.9819609413641635</v>
+        <v>0.9660997502721836</v>
       </c>
       <c r="G106" t="n" s="25">
-        <v>0.18178003084876074</v>
+        <v>0.1360134941674401</v>
       </c>
       <c r="H106" t="n" s="25">
-        <v>0.9943397705692603</v>
+        <v>0.9891000947219253</v>
       </c>
       <c r="I106" t="n" s="25">
-        <v>0.981514963075046</v>
+        <v>0.9499946226636489</v>
       </c>
       <c r="J106" t="n" s="25">
-        <v>6.253540296617605E-6</v>
+        <v>1.1753518098008743E-6</v>
       </c>
       <c r="K106" t="n" s="25">
-        <v>0.848204179536779</v>
+        <v>0.8051306034699911</v>
       </c>
       <c r="L106" t="n" s="25">
-        <v>0.004365498820730053</v>
+        <v>8.915846250541398E-4</v>
       </c>
       <c r="M106" t="n" s="25">
-        <v>2.1260484936341924E-21</v>
+        <v>1.6784511216995143E-22</v>
       </c>
       <c r="N106" t="n" s="25">
         <v>0.5</v>
@@ -4262,31 +4262,31 @@
         <v>107.0</v>
       </c>
       <c r="E107" t="n" s="25">
-        <v>0.9952321841889179</v>
+        <v>0.9939192782363315</v>
       </c>
       <c r="F107" t="n" s="25">
-        <v>0.9914487246766905</v>
+        <v>0.9810886577731547</v>
       </c>
       <c r="G107" t="n" s="25">
-        <v>0.5317193445324077</v>
+        <v>0.45197718947014986</v>
       </c>
       <c r="H107" t="n" s="25">
-        <v>0.9982575651593167</v>
+        <v>0.9951190148340602</v>
       </c>
       <c r="I107" t="n" s="25">
-        <v>0.9972816763693806</v>
+        <v>0.9902114101907581</v>
       </c>
       <c r="J107" t="n" s="25">
-        <v>0.01777378490829095</v>
+        <v>0.003507827802216832</v>
       </c>
       <c r="K107" t="n" s="25">
-        <v>0.9332576297531409</v>
+        <v>0.8681044127146378</v>
       </c>
       <c r="L107" t="n" s="25">
-        <v>0.6319171868149948</v>
+        <v>0.12304552334870102</v>
       </c>
       <c r="M107" t="n" s="25">
-        <v>1.4659208867162038E-13</v>
+        <v>3.568833308867931E-15</v>
       </c>
       <c r="N107" t="n" s="25">
         <v>0.5</v>
@@ -4297,31 +4297,31 @@
         <v>108.0</v>
       </c>
       <c r="E108" t="n" s="25">
-        <v>0.9992612861257367</v>
+        <v>0.9990183445252651</v>
       </c>
       <c r="F108" t="n" s="25">
-        <v>0.9999997062170045</v>
+        <v>0.9999983346267203</v>
       </c>
       <c r="G108" t="n" s="25">
-        <v>0.9999999999999781</v>
+        <v>0.9999999999944812</v>
       </c>
       <c r="H108" t="n" s="25">
-        <v>0.999975544854033</v>
+        <v>0.9999280977739415</v>
       </c>
       <c r="I108" t="n" s="25">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999998956</v>
       </c>
       <c r="J108" t="n" s="25">
         <v>1.0</v>
       </c>
       <c r="K108" t="n" s="25">
-        <v>0.9999460605913012</v>
+        <v>0.9997366242297858</v>
       </c>
       <c r="L108" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999990239149</v>
       </c>
       <c r="M108" t="n" s="25">
-        <v>1.0</v>
+        <v>0.9999999916581439</v>
       </c>
       <c r="N108" t="n" s="25">
         <v>0.5</v>
@@ -4332,31 +4332,31 @@
         <v>109.0</v>
       </c>
       <c r="E109" t="n" s="25">
-        <v>0.9907563258989524</v>
+        <v>0.9886771985208931</v>
       </c>
       <c r="F109" t="n" s="25">
-        <v>0.7423873214015314</v>
+        <v>0.6916507790747691</v>
       </c>
       <c r="G109" t="n" s="25">
-        <v>0.01270957295059414</v>
+        <v>0.009016158150296502</v>
       </c>
       <c r="H109" t="n" s="25">
-        <v>0.5640528110759537</v>
+        <v>0.5249342614833197</v>
       </c>
       <c r="I109" t="n" s="25">
-        <v>0.057036914686937466</v>
+        <v>0.025847349506163013</v>
       </c>
       <c r="J109" t="n" s="25">
-        <v>6.825256484991291E-13</v>
+        <v>1.3757716281216403E-13</v>
       </c>
       <c r="K109" t="n" s="25">
-        <v>0.138985709661069</v>
+        <v>0.1259908969861561</v>
       </c>
       <c r="L109" t="n" s="25">
-        <v>7.562600315378015E-10</v>
+        <v>3.097714776760702E-10</v>
       </c>
       <c r="M109" t="n" s="25">
-        <v>2.9651648435977156E-33</v>
+        <v>6.308114793967215E-34</v>
       </c>
       <c r="N109" t="n" s="25">
         <v>0.5</v>
@@ -4367,31 +4367,31 @@
         <v>110.0</v>
       </c>
       <c r="E110" t="n" s="25">
-        <v>0.9990914510156967</v>
+        <v>0.9988209996328056</v>
       </c>
       <c r="F110" t="n" s="25">
-        <v>0.997074710552855</v>
+        <v>0.9927194444512383</v>
       </c>
       <c r="G110" t="n" s="25">
-        <v>0.8760636182513117</v>
+        <v>0.7604198756055727</v>
       </c>
       <c r="H110" t="n" s="25">
-        <v>0.9977595412036815</v>
+        <v>0.9953322950238781</v>
       </c>
       <c r="I110" t="n" s="25">
-        <v>0.9962030938520052</v>
+        <v>0.9876351779602589</v>
       </c>
       <c r="J110" t="n" s="25">
-        <v>0.9532184773497941</v>
+        <v>0.3777479010148589</v>
       </c>
       <c r="K110" t="n" s="25">
-        <v>0.7371645018692953</v>
+        <v>0.7071627845252092</v>
       </c>
       <c r="L110" t="n" s="25">
-        <v>0.027985034296653288</v>
+        <v>0.011359361606508297</v>
       </c>
       <c r="M110" t="n" s="25">
-        <v>7.0815509309070955E-12</v>
+        <v>1.8054629974986426E-13</v>
       </c>
       <c r="N110" t="n" s="25">
         <v>0.5</v>
@@ -4402,31 +4402,31 @@
         <v>111.0</v>
       </c>
       <c r="E111" t="n" s="25">
-        <v>0.9989990688613227</v>
+        <v>0.9987154673842907</v>
       </c>
       <c r="F111" t="n" s="25">
-        <v>0.9819609413641635</v>
+        <v>0.9660997502721836</v>
       </c>
       <c r="G111" t="n" s="25">
-        <v>0.18177945350846686</v>
+        <v>0.1360132560042527</v>
       </c>
       <c r="H111" t="n" s="25">
-        <v>0.9917169487612278</v>
+        <v>0.9850445633666501</v>
       </c>
       <c r="I111" t="n" s="25">
-        <v>0.9815082250157697</v>
+        <v>0.9499857398595162</v>
       </c>
       <c r="J111" t="n" s="25">
-        <v>2.501425504305147E-6</v>
+        <v>4.701410554689514E-7</v>
       </c>
       <c r="K111" t="n" s="25">
-        <v>0.6971051531045412</v>
+        <v>0.6696803375782686</v>
       </c>
       <c r="L111" t="n" s="25">
-        <v>1.5185665951317057E-4</v>
+        <v>5.997543858621399E-5</v>
       </c>
       <c r="M111" t="n" s="25">
-        <v>3.297816175103146E-24</v>
+        <v>5.0252523865497E-25</v>
       </c>
       <c r="N111" t="n" s="25">
         <v>0.5</v>

</xml_diff>